<commit_message>
added products to excel file
</commit_message>
<xml_diff>
--- a/excel/producten.xlsx
+++ b/excel/producten.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25596" yWindow="0" windowWidth="25596" windowHeight="13176" tabRatio="500"/>
+    <workbookView xWindow="25600" yWindow="0" windowWidth="25600" windowHeight="13180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="163">
   <si>
     <t>productnaam</t>
   </si>
@@ -156,15 +156,9 @@
     <t>Wide angle lens</t>
   </si>
   <si>
-    <t>3-personen tent</t>
-  </si>
-  <si>
     <t>Coleman</t>
   </si>
   <si>
-    <t>Tent + maxi comfort luchtmatras</t>
-  </si>
-  <si>
     <t>Setprijs</t>
   </si>
   <si>
@@ -334,6 +328,186 @@
   </si>
   <si>
     <t>Zaklamp</t>
+  </si>
+  <si>
+    <t>Darwin 2</t>
+  </si>
+  <si>
+    <t>Tent</t>
+  </si>
+  <si>
+    <t>SEO 3</t>
+  </si>
+  <si>
+    <t>Hoofdlamp</t>
+  </si>
+  <si>
+    <t>Led Lenser</t>
+  </si>
+  <si>
+    <t>Palm tree en Flowers</t>
+  </si>
+  <si>
+    <t>Zwemshort jongens</t>
+  </si>
+  <si>
+    <t>Rumbl</t>
+  </si>
+  <si>
+    <t>Beach kids</t>
+  </si>
+  <si>
+    <t>Happy Hippie</t>
+  </si>
+  <si>
+    <t>Bikini meisjes</t>
+  </si>
+  <si>
+    <t>Lingadore</t>
+  </si>
+  <si>
+    <t>Flamingo</t>
+  </si>
+  <si>
+    <t>UV-shirt meisjes</t>
+  </si>
+  <si>
+    <t>Molo kids</t>
+  </si>
+  <si>
+    <t>Shark</t>
+  </si>
+  <si>
+    <t>UV-shirt jongens</t>
+  </si>
+  <si>
+    <t>Vigga</t>
+  </si>
+  <si>
+    <t>Jumpsuit meisjes</t>
+  </si>
+  <si>
+    <t>Name it</t>
+  </si>
+  <si>
+    <t>Assortiment zonnebrillen</t>
+  </si>
+  <si>
+    <t>met gratis zonnebescherming</t>
+  </si>
+  <si>
+    <t>Julbo</t>
+  </si>
+  <si>
+    <t>Vanaf</t>
+  </si>
+  <si>
+    <t>Snorkelset</t>
+  </si>
+  <si>
+    <t>Junior</t>
+  </si>
+  <si>
+    <t>Speedo</t>
+  </si>
+  <si>
+    <t>Strandspeelgoed</t>
+  </si>
+  <si>
+    <t>Assortiment</t>
+  </si>
+  <si>
+    <t>Quut</t>
+  </si>
+  <si>
+    <t>Assortiment slippers</t>
+  </si>
+  <si>
+    <t>Cozumel</t>
+  </si>
+  <si>
+    <t>Hoed</t>
+  </si>
+  <si>
+    <t>Barts</t>
+  </si>
+  <si>
+    <t>Beach</t>
+  </si>
+  <si>
+    <t>Ivy Jade</t>
+  </si>
+  <si>
+    <t>Bikini</t>
+  </si>
+  <si>
+    <t>Beachlife</t>
+  </si>
+  <si>
+    <t>Kachon Tee</t>
+  </si>
+  <si>
+    <t>T-shirt Heren</t>
+  </si>
+  <si>
+    <t>J&amp;J Tech</t>
+  </si>
+  <si>
+    <t>Happie Hippie</t>
+  </si>
+  <si>
+    <t>Halterneck Bikini</t>
+  </si>
+  <si>
+    <t>Mahalo</t>
+  </si>
+  <si>
+    <t>Halterneck strandjurks</t>
+  </si>
+  <si>
+    <t>Boltana</t>
+  </si>
+  <si>
+    <t>Strandjurk</t>
+  </si>
+  <si>
+    <t>Protest</t>
+  </si>
+  <si>
+    <t>Yolt</t>
+  </si>
+  <si>
+    <t>Zwemshort Heren</t>
+  </si>
+  <si>
+    <t>Assortiment teenslippers</t>
+  </si>
+  <si>
+    <t>Assortiment zonnebescherming</t>
+  </si>
+  <si>
+    <t>Skomer</t>
+  </si>
+  <si>
+    <t>T-shirt Dames</t>
+  </si>
+  <si>
+    <t>Vaude</t>
+  </si>
+  <si>
+    <t>Trekking 2+1</t>
+  </si>
+  <si>
+    <t>Masai Mara</t>
+  </si>
+  <si>
+    <t>Zambezi</t>
+  </si>
+  <si>
+    <t>Darwin 3</t>
+  </si>
+  <si>
+    <t>en Maxi Comfort Luchtmatras</t>
   </si>
 </sst>
 </file>
@@ -399,9 +573,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normaal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -735,35 +909,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W29"/>
+  <dimension ref="A1:W52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.296875" customWidth="1"/>
-    <col min="2" max="2" width="19.19921875" customWidth="1"/>
-    <col min="4" max="4" width="3.796875" customWidth="1"/>
-    <col min="5" max="5" width="4.296875" customWidth="1"/>
-    <col min="8" max="8" width="4.296875" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="3.83203125" customWidth="1"/>
+    <col min="5" max="5" width="4.33203125" customWidth="1"/>
+    <col min="8" max="8" width="4.33203125" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="5.796875" customWidth="1"/>
+    <col min="10" max="10" width="5.83203125" customWidth="1"/>
     <col min="11" max="11" width="6" customWidth="1"/>
-    <col min="12" max="12" width="4.19921875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.69921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.19921875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.19921875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="14" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.796875" customWidth="1"/>
+    <col min="21" max="21" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -834,7 +1008,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -866,7 +1040,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -898,7 +1072,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -936,7 +1110,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -968,7 +1142,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -997,7 +1171,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -1023,7 +1197,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1049,15 +1223,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>161</v>
       </c>
       <c r="B9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C9" t="s">
         <v>45</v>
-      </c>
-      <c r="C9" t="s">
-        <v>46</v>
       </c>
       <c r="F9">
         <v>159.9</v>
@@ -1066,7 +1240,7 @@
         <v>99</v>
       </c>
       <c r="I9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Q9">
         <v>1</v>
@@ -1081,21 +1255,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23">
       <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
         <v>49</v>
-      </c>
-      <c r="B10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" t="s">
-        <v>51</v>
       </c>
       <c r="G10">
         <v>19.95</v>
       </c>
       <c r="I10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="Q10">
         <v>1</v>
@@ -1110,18 +1284,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" s="1" customFormat="1">
       <c r="A11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="Q11" s="1">
         <v>1</v>
@@ -1133,15 +1307,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23">
       <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" t="s">
         <v>57</v>
-      </c>
-      <c r="B12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" t="s">
-        <v>59</v>
       </c>
       <c r="F12">
         <v>64.95</v>
@@ -1159,18 +1333,18 @@
         <v>1</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F13">
         <v>164.95</v>
@@ -1188,18 +1362,18 @@
         <v>1</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F14">
         <v>44.95</v>
@@ -1217,18 +1391,18 @@
         <v>1</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
       <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" t="s">
         <v>65</v>
-      </c>
-      <c r="B15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" t="s">
-        <v>67</v>
       </c>
       <c r="F15">
         <v>135</v>
@@ -1240,18 +1414,18 @@
         <v>1</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
       <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
         <v>65</v>
-      </c>
-      <c r="B16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" t="s">
-        <v>67</v>
       </c>
       <c r="F16">
         <v>165</v>
@@ -1263,18 +1437,18 @@
         <v>1</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23">
       <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" t="s">
         <v>65</v>
-      </c>
-      <c r="B17" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" t="s">
-        <v>67</v>
       </c>
       <c r="F17">
         <v>185</v>
@@ -1286,18 +1460,18 @@
         <v>1</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23">
       <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" t="s">
         <v>65</v>
-      </c>
-      <c r="B18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" t="s">
-        <v>67</v>
       </c>
       <c r="F18">
         <v>485</v>
@@ -1306,24 +1480,24 @@
         <v>229</v>
       </c>
       <c r="I18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R18">
         <v>1</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23">
       <c r="A19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" t="s">
         <v>71</v>
-      </c>
-      <c r="B19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" t="s">
-        <v>73</v>
       </c>
       <c r="F19">
         <v>24.95</v>
@@ -1341,18 +1515,18 @@
         <v>1</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23">
       <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" t="s">
         <v>74</v>
-      </c>
-      <c r="B20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" t="s">
-        <v>76</v>
       </c>
       <c r="F20">
         <v>79.95</v>
@@ -1373,18 +1547,18 @@
         <v>1</v>
       </c>
       <c r="W20" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B21" t="s">
         <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F21">
         <v>79</v>
@@ -1405,15 +1579,15 @@
         <v>1</v>
       </c>
       <c r="W21" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23">
       <c r="A22" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F22">
         <v>39.950000000000003</v>
@@ -1431,18 +1605,18 @@
         <v>1</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E23" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G23">
         <v>19.95</v>
@@ -1451,18 +1625,18 @@
         <v>1</v>
       </c>
       <c r="W23" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23">
       <c r="A24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" t="s">
         <v>84</v>
-      </c>
-      <c r="B24" t="s">
-        <v>85</v>
-      </c>
-      <c r="C24" t="s">
-        <v>86</v>
       </c>
       <c r="F24">
         <v>29.95</v>
@@ -1486,18 +1660,18 @@
         <v>1</v>
       </c>
       <c r="W24" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23">
+      <c r="A25" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="C25" t="s">
         <v>88</v>
-      </c>
-      <c r="B25" t="s">
-        <v>89</v>
-      </c>
-      <c r="C25" t="s">
-        <v>90</v>
       </c>
       <c r="G25">
         <v>29.95</v>
@@ -1521,18 +1695,18 @@
         <v>1</v>
       </c>
       <c r="W25" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23">
       <c r="A26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G26">
         <v>49.95</v>
@@ -1550,27 +1724,27 @@
         <v>1</v>
       </c>
       <c r="W26" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23">
       <c r="A27" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" t="s">
         <v>95</v>
-      </c>
-      <c r="B27" t="s">
-        <v>94</v>
-      </c>
-      <c r="C27" t="s">
-        <v>93</v>
-      </c>
-      <c r="E27" t="s">
-        <v>97</v>
       </c>
       <c r="G27">
         <v>94.95</v>
       </c>
       <c r="I27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O27">
         <v>1</v>
@@ -1585,18 +1759,18 @@
         <v>1</v>
       </c>
       <c r="W27" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23">
       <c r="A28" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G28">
         <v>9.9499999999999993</v>
@@ -1610,16 +1784,19 @@
       <c r="S28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W28" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23">
       <c r="A29" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C29" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F29">
         <v>9.9499999999999993</v>
@@ -1628,7 +1805,7 @@
         <v>6</v>
       </c>
       <c r="I29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="Q29">
         <v>1</v>
@@ -1637,6 +1814,529 @@
         <v>1</v>
       </c>
       <c r="S29">
+        <v>1</v>
+      </c>
+      <c r="W29" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" s="2" customFormat="1">
+      <c r="A30" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" s="2">
+        <v>74.95</v>
+      </c>
+      <c r="G30" s="2">
+        <v>49</v>
+      </c>
+      <c r="W30" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23">
+      <c r="A31" t="s">
+        <v>105</v>
+      </c>
+      <c r="B31" t="s">
+        <v>106</v>
+      </c>
+      <c r="C31" t="s">
+        <v>107</v>
+      </c>
+      <c r="F31">
+        <v>39.950000000000003</v>
+      </c>
+      <c r="G31">
+        <v>25</v>
+      </c>
+      <c r="W31" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23">
+      <c r="A32" t="s">
+        <v>108</v>
+      </c>
+      <c r="B32" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" t="s">
+        <v>110</v>
+      </c>
+      <c r="F32">
+        <v>34.950000000000003</v>
+      </c>
+      <c r="G32">
+        <v>25</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="U32">
+        <v>1</v>
+      </c>
+      <c r="W32" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23">
+      <c r="A33" t="s">
+        <v>112</v>
+      </c>
+      <c r="B33" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" t="s">
+        <v>114</v>
+      </c>
+      <c r="F33">
+        <v>24.95</v>
+      </c>
+      <c r="G33">
+        <v>19</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="O33">
+        <v>1</v>
+      </c>
+      <c r="U33">
+        <v>1</v>
+      </c>
+      <c r="W33" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
+      <c r="A34" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" t="s">
+        <v>117</v>
+      </c>
+      <c r="F34">
+        <v>27.95</v>
+      </c>
+      <c r="G34">
+        <v>19</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="O34">
+        <v>1</v>
+      </c>
+      <c r="U34">
+        <v>1</v>
+      </c>
+      <c r="W34" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23">
+      <c r="A35" t="s">
+        <v>118</v>
+      </c>
+      <c r="B35" t="s">
+        <v>119</v>
+      </c>
+      <c r="C35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F35">
+        <v>27.95</v>
+      </c>
+      <c r="G35">
+        <v>19</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="O35">
+        <v>1</v>
+      </c>
+      <c r="U35">
+        <v>1</v>
+      </c>
+      <c r="W35" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23">
+      <c r="A36" t="s">
+        <v>120</v>
+      </c>
+      <c r="B36" t="s">
+        <v>121</v>
+      </c>
+      <c r="C36" t="s">
+        <v>122</v>
+      </c>
+      <c r="G36">
+        <v>10.95</v>
+      </c>
+      <c r="O36">
+        <v>1</v>
+      </c>
+      <c r="U36">
+        <v>1</v>
+      </c>
+      <c r="W36" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23">
+      <c r="A37" t="s">
+        <v>123</v>
+      </c>
+      <c r="B37" t="s">
+        <v>124</v>
+      </c>
+      <c r="C37" t="s">
+        <v>125</v>
+      </c>
+      <c r="G37">
+        <v>29.95</v>
+      </c>
+      <c r="I37" t="s">
+        <v>126</v>
+      </c>
+      <c r="O37">
+        <v>1</v>
+      </c>
+      <c r="U37">
+        <v>1</v>
+      </c>
+      <c r="W37" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23">
+      <c r="A38" t="s">
+        <v>127</v>
+      </c>
+      <c r="B38" t="s">
+        <v>128</v>
+      </c>
+      <c r="C38" t="s">
+        <v>129</v>
+      </c>
+      <c r="F38">
+        <v>21</v>
+      </c>
+      <c r="G38">
+        <v>15</v>
+      </c>
+      <c r="O38">
+        <v>1</v>
+      </c>
+      <c r="U38">
+        <v>1</v>
+      </c>
+      <c r="W38" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23">
+      <c r="A39" t="s">
+        <v>130</v>
+      </c>
+      <c r="B39" t="s">
+        <v>131</v>
+      </c>
+      <c r="C39" t="s">
+        <v>132</v>
+      </c>
+      <c r="G39">
+        <v>7.5</v>
+      </c>
+      <c r="I39" t="s">
+        <v>126</v>
+      </c>
+      <c r="O39">
+        <v>1</v>
+      </c>
+      <c r="U39">
+        <v>1</v>
+      </c>
+      <c r="W39" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" s="1" customFormat="1">
+      <c r="A40" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="O40" s="1">
+        <v>1</v>
+      </c>
+      <c r="U40" s="1">
+        <v>1</v>
+      </c>
+      <c r="W40" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23">
+      <c r="A41" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" t="s">
+        <v>135</v>
+      </c>
+      <c r="C41" t="s">
+        <v>136</v>
+      </c>
+      <c r="F41">
+        <v>34.99</v>
+      </c>
+      <c r="G41">
+        <v>25</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
+      <c r="T41">
+        <v>1</v>
+      </c>
+      <c r="W41" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23">
+      <c r="A42" t="s">
+        <v>138</v>
+      </c>
+      <c r="B42" t="s">
+        <v>139</v>
+      </c>
+      <c r="C42" t="s">
+        <v>140</v>
+      </c>
+      <c r="F42">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="G42">
+        <v>49</v>
+      </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
+      <c r="W42" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23">
+      <c r="A43" t="s">
+        <v>141</v>
+      </c>
+      <c r="B43" t="s">
+        <v>142</v>
+      </c>
+      <c r="C43" t="s">
+        <v>143</v>
+      </c>
+      <c r="F43">
+        <v>19.95</v>
+      </c>
+      <c r="G43">
+        <v>14</v>
+      </c>
+      <c r="K43">
+        <v>1</v>
+      </c>
+      <c r="N43">
+        <v>1</v>
+      </c>
+      <c r="T43">
+        <v>1</v>
+      </c>
+      <c r="W43" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23">
+      <c r="A44" t="s">
+        <v>144</v>
+      </c>
+      <c r="B44" t="s">
+        <v>145</v>
+      </c>
+      <c r="C44" t="s">
+        <v>114</v>
+      </c>
+      <c r="F44">
+        <v>69.95</v>
+      </c>
+      <c r="G44">
+        <v>49</v>
+      </c>
+      <c r="K44">
+        <v>1</v>
+      </c>
+      <c r="M44">
+        <v>1</v>
+      </c>
+      <c r="T44">
+        <v>1</v>
+      </c>
+      <c r="W44" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23">
+      <c r="A45" t="s">
+        <v>146</v>
+      </c>
+      <c r="B45" t="s">
+        <v>147</v>
+      </c>
+      <c r="C45" t="s">
+        <v>114</v>
+      </c>
+      <c r="G45">
+        <v>39.950000000000003</v>
+      </c>
+      <c r="I45" t="s">
+        <v>25</v>
+      </c>
+      <c r="W45" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23">
+      <c r="A46" t="s">
+        <v>148</v>
+      </c>
+      <c r="B46" t="s">
+        <v>149</v>
+      </c>
+      <c r="C46" t="s">
+        <v>150</v>
+      </c>
+      <c r="F46">
+        <v>49.95</v>
+      </c>
+      <c r="G46">
+        <v>35</v>
+      </c>
+      <c r="K46">
+        <v>1</v>
+      </c>
+      <c r="M46">
+        <v>1</v>
+      </c>
+      <c r="W46" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23">
+      <c r="A47" t="s">
+        <v>151</v>
+      </c>
+      <c r="B47" t="s">
+        <v>152</v>
+      </c>
+      <c r="C47" t="s">
+        <v>150</v>
+      </c>
+      <c r="F47">
+        <v>49.95</v>
+      </c>
+      <c r="G47">
+        <v>35</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <v>1</v>
+      </c>
+      <c r="W47" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" s="1" customFormat="1">
+      <c r="A48" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="W48" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" s="1" customFormat="1">
+      <c r="A49" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="W49" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23">
+      <c r="A50" t="s">
+        <v>155</v>
+      </c>
+      <c r="B50" t="s">
+        <v>156</v>
+      </c>
+      <c r="C50" t="s">
+        <v>157</v>
+      </c>
+      <c r="G50">
+        <v>36.950000000000003</v>
+      </c>
+      <c r="L50">
+        <v>1</v>
+      </c>
+      <c r="W50" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23">
+      <c r="A51" t="s">
+        <v>159</v>
+      </c>
+      <c r="B51" t="s">
+        <v>156</v>
+      </c>
+      <c r="C51" t="s">
+        <v>88</v>
+      </c>
+      <c r="G51">
+        <v>34.950000000000003</v>
+      </c>
+      <c r="L51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23">
+      <c r="A52" t="s">
+        <v>160</v>
+      </c>
+      <c r="B52" t="s">
+        <v>156</v>
+      </c>
+      <c r="C52" t="s">
+        <v>88</v>
+      </c>
+      <c r="G52">
+        <v>29.95</v>
+      </c>
+      <c r="L52">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added missing numbers in 'volgorde'
</commit_message>
<xml_diff>
--- a/excel/producten.xlsx
+++ b/excel/producten.xlsx
@@ -1547,8 +1547,8 @@
   <dimension ref="A1:AA116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D116" sqref="D116"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y111" sqref="Y111:Y116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1724,7 +1724,7 @@
         <v>29</v>
       </c>
       <c r="Y3" s="2">
-        <f>Y2+3</f>
+        <f t="shared" ref="Y3:Y34" si="0">Y2+3</f>
         <v>4</v>
       </c>
       <c r="Z3" s="2"/>
@@ -1770,7 +1770,7 @@
         <v>29</v>
       </c>
       <c r="Y4" s="2">
-        <f>Y3+3</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="Z4" s="2"/>
@@ -1813,7 +1813,7 @@
         <v>29</v>
       </c>
       <c r="Y5" s="2">
-        <f>Y4+3</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="Z5" s="2"/>
@@ -1844,7 +1844,7 @@
         <v>29</v>
       </c>
       <c r="Y6" s="2">
-        <f>Y5+3</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="Z6" s="2"/>
@@ -1878,7 +1878,7 @@
         <v>29</v>
       </c>
       <c r="Y7" s="2">
-        <f>Y6+3</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="Z7" s="2"/>
@@ -1912,7 +1912,7 @@
         <v>29</v>
       </c>
       <c r="Y8" s="2">
-        <f>Y7+3</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="Z8" s="2"/>
@@ -1952,7 +1952,7 @@
         <v>29</v>
       </c>
       <c r="Y9" s="2">
-        <f>Y8+3</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="Z9" s="2"/>
@@ -1992,7 +1992,7 @@
         <v>29</v>
       </c>
       <c r="Y10" s="2">
-        <f>Y9+3</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="Z10" s="2"/>
@@ -2025,7 +2025,7 @@
         <v>29</v>
       </c>
       <c r="Y11" s="2">
-        <f>Y10+3</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="Z11" s="2"/>
@@ -2065,7 +2065,7 @@
         <v>71</v>
       </c>
       <c r="Y12" s="2">
-        <f>Y11+3</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="Z12" s="2"/>
@@ -2105,7 +2105,7 @@
         <v>71</v>
       </c>
       <c r="Y13" s="2">
-        <f>Y12+3</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="Z13" s="2"/>
@@ -2145,7 +2145,7 @@
         <v>71</v>
       </c>
       <c r="Y14" s="2">
-        <f>Y13+3</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="Z14" s="2"/>
@@ -2179,7 +2179,7 @@
         <v>71</v>
       </c>
       <c r="Y15" s="2">
-        <f>Y14+3</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="Z15" s="2"/>
@@ -2213,7 +2213,7 @@
         <v>71</v>
       </c>
       <c r="Y16" s="2">
-        <f>Y15+3</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="Z16" s="2"/>
@@ -2247,7 +2247,7 @@
         <v>71</v>
       </c>
       <c r="Y17" s="2">
-        <f>Y16+3</f>
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="Z17" s="2"/>
@@ -2281,7 +2281,7 @@
         <v>71</v>
       </c>
       <c r="Y18" s="2">
-        <f>Y17+3</f>
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="Z18" s="2"/>
@@ -2321,7 +2321,7 @@
         <v>71</v>
       </c>
       <c r="Y19" s="2">
-        <f>Y18+3</f>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="Z19" s="2"/>
@@ -2364,7 +2364,7 @@
         <v>71</v>
       </c>
       <c r="Y20" s="2">
-        <f>Y19+3</f>
+        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="Z20" s="2"/>
@@ -2404,7 +2404,7 @@
         <v>71</v>
       </c>
       <c r="Y21" s="2">
-        <f>Y20+3</f>
+        <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="Z21" s="2"/>
@@ -2441,7 +2441,7 @@
         <v>71</v>
       </c>
       <c r="Y22" s="2">
-        <f>Y21+3</f>
+        <f t="shared" si="0"/>
         <v>61</v>
       </c>
       <c r="Z22" s="2"/>
@@ -2472,7 +2472,7 @@
         <v>71</v>
       </c>
       <c r="Y23" s="2">
-        <f>Y22+3</f>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="Z23" s="2"/>
@@ -2518,7 +2518,7 @@
         <v>81</v>
       </c>
       <c r="Y24" s="2">
-        <f>Y23+3</f>
+        <f t="shared" si="0"/>
         <v>67</v>
       </c>
       <c r="Z24" s="2"/>
@@ -2564,7 +2564,7 @@
         <v>81</v>
       </c>
       <c r="Y25" s="2">
-        <f>Y24+3</f>
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="Z25" s="2"/>
@@ -2604,7 +2604,7 @@
         <v>81</v>
       </c>
       <c r="Y26" s="2">
-        <f>Y25+3</f>
+        <f t="shared" si="0"/>
         <v>73</v>
       </c>
       <c r="Z26" s="2"/>
@@ -2647,7 +2647,7 @@
         <v>81</v>
       </c>
       <c r="Y27" s="2">
-        <f>Y26+3</f>
+        <f t="shared" si="0"/>
         <v>76</v>
       </c>
       <c r="Z27" s="2"/>
@@ -2684,7 +2684,7 @@
         <v>81</v>
       </c>
       <c r="Y28" s="2">
-        <f>Y27+3</f>
+        <f t="shared" si="0"/>
         <v>79</v>
       </c>
       <c r="Z28" s="2"/>
@@ -2727,7 +2727,7 @@
         <v>81</v>
       </c>
       <c r="Y29" s="2">
-        <f>Y28+3</f>
+        <f t="shared" si="0"/>
         <v>82</v>
       </c>
       <c r="Z29" s="2"/>
@@ -2769,7 +2769,7 @@
         <v>81</v>
       </c>
       <c r="Y30" s="2">
-        <f>Y29+3</f>
+        <f t="shared" si="0"/>
         <v>85</v>
       </c>
       <c r="AA30" s="2" t="s">
@@ -2799,7 +2799,7 @@
         <v>81</v>
       </c>
       <c r="Y31" s="2">
-        <f>Y30+3</f>
+        <f t="shared" si="0"/>
         <v>88</v>
       </c>
       <c r="Z31" s="2"/>
@@ -2836,7 +2836,7 @@
         <v>106</v>
       </c>
       <c r="Y32" s="2">
-        <f>Y31+3</f>
+        <f t="shared" si="0"/>
         <v>91</v>
       </c>
       <c r="Z32" s="2"/>
@@ -2873,7 +2873,7 @@
         <v>106</v>
       </c>
       <c r="Y33" s="2">
-        <f>Y32+3</f>
+        <f t="shared" si="0"/>
         <v>94</v>
       </c>
       <c r="Z33" s="2"/>
@@ -2910,7 +2910,7 @@
         <v>106</v>
       </c>
       <c r="Y34" s="2">
-        <f>Y33+3</f>
+        <f t="shared" si="0"/>
         <v>97</v>
       </c>
       <c r="Z34" s="2"/>
@@ -2947,7 +2947,7 @@
         <v>106</v>
       </c>
       <c r="Y35" s="2">
-        <f>Y34+3</f>
+        <f t="shared" ref="Y35:Y66" si="1">Y34+3</f>
         <v>100</v>
       </c>
       <c r="Z35" s="2"/>
@@ -2978,7 +2978,7 @@
         <v>106</v>
       </c>
       <c r="Y36" s="2">
-        <f>Y35+3</f>
+        <f t="shared" si="1"/>
         <v>103</v>
       </c>
       <c r="Z36" s="2"/>
@@ -3012,7 +3012,7 @@
         <v>106</v>
       </c>
       <c r="Y37" s="2">
-        <f>Y36+3</f>
+        <f t="shared" si="1"/>
         <v>106</v>
       </c>
       <c r="Z37" s="2"/>
@@ -3046,7 +3046,7 @@
         <v>106</v>
       </c>
       <c r="Y38" s="2">
-        <f>Y37+3</f>
+        <f t="shared" si="1"/>
         <v>109</v>
       </c>
       <c r="Z38" s="2"/>
@@ -3080,7 +3080,7 @@
         <v>106</v>
       </c>
       <c r="Y39" s="2">
-        <f>Y38+3</f>
+        <f t="shared" si="1"/>
         <v>112</v>
       </c>
       <c r="Z39" s="2"/>
@@ -3104,7 +3104,7 @@
         <v>106</v>
       </c>
       <c r="Y40" s="2">
-        <f>Y39+3</f>
+        <f t="shared" si="1"/>
         <v>115</v>
       </c>
       <c r="Z40" s="2"/>
@@ -3141,7 +3141,7 @@
         <v>132</v>
       </c>
       <c r="Y41" s="2">
-        <f>Y40+3</f>
+        <f t="shared" si="1"/>
         <v>118</v>
       </c>
       <c r="Z41" s="2"/>
@@ -3175,7 +3175,7 @@
         <v>132</v>
       </c>
       <c r="Y42" s="2">
-        <f>Y41+3</f>
+        <f t="shared" si="1"/>
         <v>121</v>
       </c>
       <c r="Z42" s="2"/>
@@ -3215,7 +3215,7 @@
         <v>132</v>
       </c>
       <c r="Y43" s="2">
-        <f>Y42+3</f>
+        <f t="shared" si="1"/>
         <v>124</v>
       </c>
       <c r="Z43" s="2"/>
@@ -3252,7 +3252,7 @@
         <v>132</v>
       </c>
       <c r="Y44" s="2">
-        <f>Y43+3</f>
+        <f t="shared" si="1"/>
         <v>127</v>
       </c>
       <c r="Z44" s="2"/>
@@ -3283,7 +3283,7 @@
         <v>132</v>
       </c>
       <c r="Y45" s="2">
-        <f>Y44+3</f>
+        <f t="shared" si="1"/>
         <v>130</v>
       </c>
       <c r="Z45" s="2"/>
@@ -3320,7 +3320,7 @@
         <v>132</v>
       </c>
       <c r="Y46" s="2">
-        <f>Y45+3</f>
+        <f t="shared" si="1"/>
         <v>133</v>
       </c>
       <c r="Z46" s="2"/>
@@ -3360,7 +3360,7 @@
         <v>132</v>
       </c>
       <c r="Y47" s="2">
-        <f>Y46+3</f>
+        <f t="shared" si="1"/>
         <v>136</v>
       </c>
       <c r="Z47" s="2"/>
@@ -3381,7 +3381,7 @@
         <v>132</v>
       </c>
       <c r="Y48" s="2">
-        <f>Y47+3</f>
+        <f t="shared" si="1"/>
         <v>139</v>
       </c>
       <c r="Z48" s="2"/>
@@ -3402,7 +3402,7 @@
         <v>132</v>
       </c>
       <c r="Y49" s="2">
-        <f>Y48+3</f>
+        <f t="shared" si="1"/>
         <v>142</v>
       </c>
       <c r="Z49" s="2"/>
@@ -3439,7 +3439,7 @@
         <v>153</v>
       </c>
       <c r="Y50" s="2">
-        <f>Y49+3</f>
+        <f t="shared" si="1"/>
         <v>145</v>
       </c>
       <c r="Z50" s="2"/>
@@ -3473,7 +3473,7 @@
         <v>153</v>
       </c>
       <c r="Y51" s="2">
-        <f>Y50+3</f>
+        <f t="shared" si="1"/>
         <v>148</v>
       </c>
       <c r="Z51" s="2"/>
@@ -3507,7 +3507,7 @@
         <v>153</v>
       </c>
       <c r="Y52" s="2">
-        <f>Y51+3</f>
+        <f t="shared" si="1"/>
         <v>151</v>
       </c>
       <c r="Z52" s="2"/>
@@ -3541,7 +3541,7 @@
         <v>153</v>
       </c>
       <c r="Y53" s="2">
-        <f>Y52+3</f>
+        <f t="shared" si="1"/>
         <v>154</v>
       </c>
       <c r="Z53" s="2"/>
@@ -3575,7 +3575,7 @@
         <v>153</v>
       </c>
       <c r="Y54" s="2">
-        <f>Y53+3</f>
+        <f t="shared" si="1"/>
         <v>157</v>
       </c>
       <c r="Z54" s="2"/>
@@ -3609,7 +3609,7 @@
         <v>153</v>
       </c>
       <c r="Y55" s="2">
-        <f>Y54+3</f>
+        <f t="shared" si="1"/>
         <v>160</v>
       </c>
       <c r="Z55" s="2"/>
@@ -3643,7 +3643,7 @@
         <v>153</v>
       </c>
       <c r="Y56" s="2">
-        <f>Y55+3</f>
+        <f t="shared" si="1"/>
         <v>163</v>
       </c>
       <c r="Z56" s="2"/>
@@ -3677,7 +3677,7 @@
         <v>153</v>
       </c>
       <c r="Y57" s="2">
-        <f>Y56+3</f>
+        <f t="shared" si="1"/>
         <v>166</v>
       </c>
       <c r="Z57" s="2"/>
@@ -3711,7 +3711,7 @@
         <v>153</v>
       </c>
       <c r="Y58" s="2">
-        <f>Y57+3</f>
+        <f t="shared" si="1"/>
         <v>169</v>
       </c>
       <c r="Z58" s="2"/>
@@ -3745,7 +3745,7 @@
         <v>153</v>
       </c>
       <c r="Y59" s="2">
-        <f>Y58+3</f>
+        <f t="shared" si="1"/>
         <v>172</v>
       </c>
       <c r="Z59" s="2"/>
@@ -3779,7 +3779,7 @@
         <v>153</v>
       </c>
       <c r="Y60" s="2">
-        <f>Y59+3</f>
+        <f t="shared" si="1"/>
         <v>175</v>
       </c>
       <c r="Z60" s="2"/>
@@ -3813,7 +3813,7 @@
         <v>153</v>
       </c>
       <c r="Y61" s="2">
-        <f>Y60+3</f>
+        <f t="shared" si="1"/>
         <v>178</v>
       </c>
       <c r="Z61" s="2"/>
@@ -3847,7 +3847,7 @@
         <v>153</v>
       </c>
       <c r="Y62" s="2">
-        <f>Y61+3</f>
+        <f t="shared" si="1"/>
         <v>181</v>
       </c>
       <c r="Z62" s="2"/>
@@ -3881,7 +3881,7 @@
         <v>153</v>
       </c>
       <c r="Y63" s="2">
-        <f>Y62+3</f>
+        <f t="shared" si="1"/>
         <v>184</v>
       </c>
       <c r="Z63" s="2"/>
@@ -3915,7 +3915,7 @@
         <v>153</v>
       </c>
       <c r="Y64" s="2">
-        <f>Y63+3</f>
+        <f t="shared" si="1"/>
         <v>187</v>
       </c>
       <c r="Z64" s="2"/>
@@ -3949,7 +3949,7 @@
         <v>153</v>
       </c>
       <c r="Y65" s="2">
-        <f>Y64+3</f>
+        <f t="shared" si="1"/>
         <v>190</v>
       </c>
       <c r="Z65" s="2"/>
@@ -3983,7 +3983,7 @@
         <v>153</v>
       </c>
       <c r="Y66" s="2">
-        <f>Y65+3</f>
+        <f t="shared" si="1"/>
         <v>193</v>
       </c>
       <c r="Z66" s="2"/>
@@ -4017,7 +4017,7 @@
         <v>153</v>
       </c>
       <c r="Y67" s="2">
-        <f>Y66+3</f>
+        <f t="shared" ref="Y67:Y98" si="2">Y66+3</f>
         <v>196</v>
       </c>
       <c r="Z67" s="2"/>
@@ -4051,7 +4051,7 @@
         <v>153</v>
       </c>
       <c r="Y68" s="2">
-        <f>Y67+3</f>
+        <f t="shared" si="2"/>
         <v>199</v>
       </c>
       <c r="Z68" s="2"/>
@@ -4085,7 +4085,7 @@
         <v>153</v>
       </c>
       <c r="Y69" s="2">
-        <f>Y68+3</f>
+        <f t="shared" si="2"/>
         <v>202</v>
       </c>
       <c r="Z69" s="2"/>
@@ -4119,7 +4119,7 @@
         <v>153</v>
       </c>
       <c r="Y70" s="2">
-        <f>Y69+3</f>
+        <f t="shared" si="2"/>
         <v>205</v>
       </c>
       <c r="Z70" s="2"/>
@@ -4153,7 +4153,7 @@
         <v>153</v>
       </c>
       <c r="Y71" s="2">
-        <f>Y70+3</f>
+        <f t="shared" si="2"/>
         <v>208</v>
       </c>
       <c r="Z71" s="2"/>
@@ -4187,7 +4187,7 @@
         <v>153</v>
       </c>
       <c r="Y72" s="2">
-        <f>Y71+3</f>
+        <f t="shared" si="2"/>
         <v>211</v>
       </c>
       <c r="Z72" s="2"/>
@@ -4221,7 +4221,7 @@
         <v>153</v>
       </c>
       <c r="Y73" s="2">
-        <f>Y72+3</f>
+        <f t="shared" si="2"/>
         <v>214</v>
       </c>
       <c r="Z73" s="2"/>
@@ -4255,7 +4255,7 @@
         <v>153</v>
       </c>
       <c r="Y74" s="2">
-        <f>Y73+3</f>
+        <f t="shared" si="2"/>
         <v>217</v>
       </c>
       <c r="Z74" s="2"/>
@@ -4289,7 +4289,7 @@
         <v>153</v>
       </c>
       <c r="Y75" s="2">
-        <f>Y74+3</f>
+        <f t="shared" si="2"/>
         <v>220</v>
       </c>
       <c r="Z75" s="2"/>
@@ -4323,7 +4323,7 @@
         <v>153</v>
       </c>
       <c r="Y76" s="2">
-        <f>Y75+3</f>
+        <f t="shared" si="2"/>
         <v>223</v>
       </c>
       <c r="Z76" s="2"/>
@@ -4357,7 +4357,7 @@
         <v>153</v>
       </c>
       <c r="Y77" s="2">
-        <f>Y76+3</f>
+        <f t="shared" si="2"/>
         <v>226</v>
       </c>
       <c r="Z77" s="2"/>
@@ -4391,7 +4391,7 @@
         <v>153</v>
       </c>
       <c r="Y78" s="2">
-        <f>Y77+3</f>
+        <f t="shared" si="2"/>
         <v>229</v>
       </c>
       <c r="Z78" s="2"/>
@@ -4425,7 +4425,7 @@
         <v>153</v>
       </c>
       <c r="Y79" s="2">
-        <f>Y78+3</f>
+        <f t="shared" si="2"/>
         <v>232</v>
       </c>
       <c r="Z79" s="2"/>
@@ -4462,7 +4462,7 @@
         <v>190</v>
       </c>
       <c r="Y80" s="2">
-        <f>Y79+3</f>
+        <f t="shared" si="2"/>
         <v>235</v>
       </c>
       <c r="Z80" s="2"/>
@@ -4499,7 +4499,7 @@
         <v>190</v>
       </c>
       <c r="Y81" s="2">
-        <f>Y80+3</f>
+        <f t="shared" si="2"/>
         <v>238</v>
       </c>
       <c r="Z81" s="2"/>
@@ -4536,7 +4536,7 @@
         <v>190</v>
       </c>
       <c r="Y82" s="2">
-        <f>Y81+3</f>
+        <f t="shared" si="2"/>
         <v>241</v>
       </c>
       <c r="Z82" s="2"/>
@@ -4570,7 +4570,7 @@
         <v>190</v>
       </c>
       <c r="Y83" s="2">
-        <f>Y82+3</f>
+        <f t="shared" si="2"/>
         <v>244</v>
       </c>
       <c r="Z83" s="2"/>
@@ -4587,7 +4587,7 @@
         <v>190</v>
       </c>
       <c r="Y84" s="2">
-        <f>Y83+3</f>
+        <f t="shared" si="2"/>
         <v>247</v>
       </c>
       <c r="Z84" s="2"/>
@@ -4605,7 +4605,7 @@
         <v>190</v>
       </c>
       <c r="Y85" s="2">
-        <f>Y84+3</f>
+        <f t="shared" si="2"/>
         <v>250</v>
       </c>
       <c r="Z85" s="2"/>
@@ -4640,7 +4640,7 @@
         <v>190</v>
       </c>
       <c r="Y86" s="2">
-        <f>Y85+3</f>
+        <f t="shared" si="2"/>
         <v>253</v>
       </c>
       <c r="Z86" s="2"/>
@@ -4674,7 +4674,7 @@
         <v>204</v>
       </c>
       <c r="Y87" s="2">
-        <f>Y86+3</f>
+        <f t="shared" si="2"/>
         <v>256</v>
       </c>
       <c r="Z87" s="2"/>
@@ -4708,7 +4708,7 @@
         <v>204</v>
       </c>
       <c r="Y88" s="2">
-        <f>Y87+3</f>
+        <f t="shared" si="2"/>
         <v>259</v>
       </c>
       <c r="Z88" s="2"/>
@@ -4742,7 +4742,7 @@
         <v>204</v>
       </c>
       <c r="Y89" s="2">
-        <f>Y88+3</f>
+        <f t="shared" si="2"/>
         <v>262</v>
       </c>
       <c r="Z89" s="2"/>
@@ -4776,7 +4776,7 @@
         <v>204</v>
       </c>
       <c r="Y90" s="2">
-        <f>Y89+3</f>
+        <f t="shared" si="2"/>
         <v>265</v>
       </c>
       <c r="Z90" s="2"/>
@@ -4804,7 +4804,7 @@
         <v>204</v>
       </c>
       <c r="Y91" s="2">
-        <f>Y90+3</f>
+        <f t="shared" si="2"/>
         <v>268</v>
       </c>
       <c r="Z91" s="2"/>
@@ -4829,7 +4829,7 @@
         <v>204</v>
       </c>
       <c r="Y92" s="2">
-        <f>Y91+3</f>
+        <f t="shared" si="2"/>
         <v>271</v>
       </c>
       <c r="Z92" s="2"/>
@@ -4860,7 +4860,7 @@
         <v>204</v>
       </c>
       <c r="Y93" s="2">
-        <f>Y92+3</f>
+        <f t="shared" si="2"/>
         <v>274</v>
       </c>
       <c r="Z93" s="2"/>
@@ -4888,7 +4888,7 @@
         <v>204</v>
       </c>
       <c r="Y94" s="2">
-        <f>Y93+3</f>
+        <f t="shared" si="2"/>
         <v>277</v>
       </c>
       <c r="Z94" s="2"/>
@@ -4916,7 +4916,7 @@
         <v>204</v>
       </c>
       <c r="Y95" s="2">
-        <f>Y94+3</f>
+        <f t="shared" si="2"/>
         <v>280</v>
       </c>
       <c r="Z95" s="2"/>
@@ -4944,7 +4944,7 @@
         <v>204</v>
       </c>
       <c r="Y96" s="2">
-        <f>Y95+3</f>
+        <f t="shared" si="2"/>
         <v>283</v>
       </c>
       <c r="Z96" s="2"/>
@@ -4972,7 +4972,7 @@
         <v>204</v>
       </c>
       <c r="Y97" s="2">
-        <f>Y96+3</f>
+        <f t="shared" si="2"/>
         <v>286</v>
       </c>
       <c r="Z97" s="2"/>
@@ -5003,7 +5003,7 @@
         <v>204</v>
       </c>
       <c r="Y98" s="2">
-        <f>Y97+3</f>
+        <f t="shared" si="2"/>
         <v>289</v>
       </c>
       <c r="Z98" s="2"/>
@@ -5034,7 +5034,7 @@
         <v>233</v>
       </c>
       <c r="Y99" s="2">
-        <f>Y98+3</f>
+        <f t="shared" ref="Y99:Y116" si="3">Y98+3</f>
         <v>292</v>
       </c>
       <c r="Z99" s="2"/>
@@ -5065,7 +5065,7 @@
         <v>233</v>
       </c>
       <c r="Y100" s="2">
-        <f>Y99+3</f>
+        <f t="shared" si="3"/>
         <v>295</v>
       </c>
       <c r="Z100" s="2"/>
@@ -5096,7 +5096,7 @@
         <v>233</v>
       </c>
       <c r="Y101" s="2">
-        <f>Y100+3</f>
+        <f t="shared" si="3"/>
         <v>298</v>
       </c>
       <c r="Z101" s="2"/>
@@ -5124,7 +5124,7 @@
         <v>233</v>
       </c>
       <c r="Y102" s="2">
-        <f>Y101+3</f>
+        <f t="shared" si="3"/>
         <v>301</v>
       </c>
       <c r="Z102" s="2"/>
@@ -5152,7 +5152,7 @@
         <v>233</v>
       </c>
       <c r="Y103" s="2">
-        <f>Y102+3</f>
+        <f t="shared" si="3"/>
         <v>304</v>
       </c>
       <c r="Z103" s="2"/>
@@ -5180,7 +5180,7 @@
         <v>233</v>
       </c>
       <c r="Y104" s="2">
-        <f>Y103+3</f>
+        <f t="shared" si="3"/>
         <v>307</v>
       </c>
       <c r="Z104" s="2"/>
@@ -5211,7 +5211,7 @@
         <v>233</v>
       </c>
       <c r="Y105" s="2">
-        <f>Y104+3</f>
+        <f t="shared" si="3"/>
         <v>310</v>
       </c>
       <c r="Z105" s="2"/>
@@ -5239,7 +5239,7 @@
         <v>233</v>
       </c>
       <c r="Y106" s="2">
-        <f>Y105+3</f>
+        <f t="shared" si="3"/>
         <v>313</v>
       </c>
       <c r="Z106" s="2"/>
@@ -5270,7 +5270,7 @@
         <v>233</v>
       </c>
       <c r="Y107" s="2">
-        <f>Y106+3</f>
+        <f t="shared" si="3"/>
         <v>316</v>
       </c>
       <c r="Z107" s="2"/>
@@ -5298,7 +5298,7 @@
         <v>259</v>
       </c>
       <c r="Y108" s="2">
-        <f>Y107+3</f>
+        <f t="shared" si="3"/>
         <v>319</v>
       </c>
       <c r="Z108" s="2"/>
@@ -5326,7 +5326,7 @@
         <v>259</v>
       </c>
       <c r="Y109" s="2">
-        <f>Y108+3</f>
+        <f t="shared" si="3"/>
         <v>322</v>
       </c>
       <c r="Z109" s="2"/>
@@ -5354,7 +5354,7 @@
         <v>259</v>
       </c>
       <c r="Y110" s="2">
-        <f>Y109+3</f>
+        <f t="shared" si="3"/>
         <v>325</v>
       </c>
       <c r="Z110" s="2"/>
@@ -5382,7 +5382,7 @@
         <v>259</v>
       </c>
       <c r="Y111" s="2">
-        <f>Y110+3</f>
+        <f t="shared" si="3"/>
         <v>328</v>
       </c>
       <c r="Z111" s="2"/>
@@ -5406,8 +5406,12 @@
       <c r="X112" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="113" spans="1:24">
+      <c r="Y112" s="2">
+        <f t="shared" si="3"/>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="113" spans="1:25">
       <c r="A113" t="s">
         <v>266</v>
       </c>
@@ -5429,8 +5433,12 @@
       <c r="X113" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="114" spans="1:24">
+      <c r="Y113" s="2">
+        <f t="shared" si="3"/>
+        <v>334</v>
+      </c>
+    </row>
+    <row r="114" spans="1:25">
       <c r="A114" t="s">
         <v>265</v>
       </c>
@@ -5452,8 +5460,12 @@
       <c r="X114" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="115" spans="1:24">
+      <c r="Y114" s="2">
+        <f t="shared" si="3"/>
+        <v>337</v>
+      </c>
+    </row>
+    <row r="115" spans="1:25">
       <c r="A115" t="s">
         <v>268</v>
       </c>
@@ -5469,8 +5481,12 @@
       <c r="X115" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="116" spans="1:24">
+      <c r="Y115" s="2">
+        <f t="shared" si="3"/>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="116" spans="1:25">
       <c r="A116" t="s">
         <v>270</v>
       </c>
@@ -5491,6 +5507,10 @@
       </c>
       <c r="X116" t="s">
         <v>259</v>
+      </c>
+      <c r="Y116" s="2">
+        <f t="shared" si="3"/>
+        <v>343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
producten.xlsx assign products to categories
</commit_message>
<xml_diff>
--- a/excel/producten.xlsx
+++ b/excel/producten.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="0" windowWidth="25380" windowHeight="26500" tabRatio="500"/>
+    <workbookView xWindow="2700" yWindow="0" windowWidth="25380" windowHeight="13176" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="370">
   <si>
     <t>productnaam</t>
   </si>
@@ -1208,9 +1208,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Normaal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1546,33 +1546,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y111" sqref="Y111:Y116"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA54" sqref="AA54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
-    <col min="4" max="4" width="62.83203125" customWidth="1"/>
-    <col min="5" max="5" width="4.33203125" customWidth="1"/>
-    <col min="8" max="8" width="4.33203125" customWidth="1"/>
-    <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="11" width="5.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.296875" customWidth="1"/>
+    <col min="2" max="2" width="28.296875" customWidth="1"/>
+    <col min="4" max="4" width="51.09765625" customWidth="1"/>
+    <col min="5" max="5" width="4.296875" customWidth="1"/>
+    <col min="8" max="8" width="4.296875" customWidth="1"/>
+    <col min="9" max="9" width="10.09765625" customWidth="1"/>
+    <col min="10" max="11" width="5.796875" customWidth="1"/>
     <col min="12" max="12" width="6" style="3" customWidth="1"/>
-    <col min="13" max="13" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.19921875" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.69921875" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.83203125" customWidth="1"/>
+    <col min="17" max="17" width="7.19921875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.19921875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.09765625" customWidth="1"/>
+    <col min="22" max="22" width="11.19921875" customWidth="1"/>
+    <col min="23" max="23" width="6.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1652,7 +1653,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="2" customFormat="1">
+    <row r="2" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -1688,11 +1689,8 @@
       <c r="Y2" s="2">
         <v>1</v>
       </c>
-      <c r="AA2" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27">
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1728,11 +1726,8 @@
         <v>4</v>
       </c>
       <c r="Z3" s="2"/>
-      <c r="AA3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27">
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1774,11 +1769,8 @@
         <v>7</v>
       </c>
       <c r="Z4" s="2"/>
-      <c r="AA4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27">
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1817,11 +1809,8 @@
         <v>10</v>
       </c>
       <c r="Z5" s="2"/>
-      <c r="AA5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27">
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1836,6 +1825,12 @@
       </c>
       <c r="G6">
         <v>19</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
       </c>
       <c r="S6">
         <v>1</v>
@@ -1848,11 +1843,8 @@
         <v>13</v>
       </c>
       <c r="Z6" s="2"/>
-      <c r="AA6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27">
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1867,6 +1859,12 @@
       </c>
       <c r="G7">
         <v>29.95</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
       </c>
       <c r="R7">
         <v>1</v>
@@ -1882,11 +1880,8 @@
         <v>16</v>
       </c>
       <c r="Z7" s="2"/>
-      <c r="AA7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27">
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1901,6 +1896,12 @@
       </c>
       <c r="G8">
         <v>44.95</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
       </c>
       <c r="R8">
         <v>1</v>
@@ -1916,11 +1917,8 @@
         <v>19</v>
       </c>
       <c r="Z8" s="2"/>
-      <c r="AA8" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27">
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>156</v>
       </c>
@@ -1938,6 +1936,12 @@
       </c>
       <c r="I9" t="s">
         <v>43</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
       </c>
       <c r="R9">
         <v>1</v>
@@ -1956,11 +1960,8 @@
         <v>22</v>
       </c>
       <c r="Z9" s="2"/>
-      <c r="AA9" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27">
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -1978,6 +1979,12 @@
       </c>
       <c r="I10" t="s">
         <v>47</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
       </c>
       <c r="R10">
         <v>1</v>
@@ -1996,11 +2003,8 @@
         <v>25</v>
       </c>
       <c r="Z10" s="2"/>
-      <c r="AA10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" s="1" customFormat="1">
+    </row>
+    <row r="11" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>48</v>
       </c>
@@ -2015,6 +2019,12 @@
       </c>
       <c r="L11" s="3"/>
       <c r="M11" s="4"/>
+      <c r="N11" s="1">
+        <v>1</v>
+      </c>
+      <c r="O11" s="1">
+        <v>1</v>
+      </c>
       <c r="R11" s="1">
         <v>1</v>
       </c>
@@ -2029,11 +2039,8 @@
         <v>28</v>
       </c>
       <c r="Z11" s="2"/>
-      <c r="AA11" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27">
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -2069,11 +2076,8 @@
         <v>31</v>
       </c>
       <c r="Z12" s="2"/>
-      <c r="AA12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27">
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -2091,6 +2095,12 @@
       </c>
       <c r="G13">
         <v>99</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
       </c>
       <c r="R13">
         <v>1</v>
@@ -2109,11 +2119,8 @@
         <v>34</v>
       </c>
       <c r="Z13" s="2"/>
-      <c r="AA13" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27">
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -2131,6 +2138,12 @@
       </c>
       <c r="G14">
         <v>29</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
       </c>
       <c r="R14">
         <v>1</v>
@@ -2149,11 +2162,8 @@
         <v>37</v>
       </c>
       <c r="Z14" s="2"/>
-      <c r="AA14" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27">
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -2171,6 +2181,12 @@
       </c>
       <c r="G15">
         <v>85</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
       </c>
       <c r="S15">
         <v>1</v>
@@ -2183,11 +2199,8 @@
         <v>40</v>
       </c>
       <c r="Z15" s="2"/>
-      <c r="AA15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27">
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -2205,6 +2218,12 @@
       </c>
       <c r="G16">
         <v>105</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
       </c>
       <c r="S16">
         <v>1</v>
@@ -2217,11 +2236,8 @@
         <v>43</v>
       </c>
       <c r="Z16" s="2"/>
-      <c r="AA16" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27">
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -2239,6 +2255,12 @@
       </c>
       <c r="G17">
         <v>115</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
       </c>
       <c r="S17">
         <v>1</v>
@@ -2251,11 +2273,8 @@
         <v>46</v>
       </c>
       <c r="Z17" s="2"/>
-      <c r="AA17" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="18" spans="1:27">
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>59</v>
       </c>
@@ -2273,6 +2292,12 @@
       </c>
       <c r="I18" t="s">
         <v>43</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
       </c>
       <c r="S18">
         <v>1</v>
@@ -2285,11 +2310,8 @@
         <v>49</v>
       </c>
       <c r="Z18" s="2"/>
-      <c r="AA18" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27">
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -2307,6 +2329,12 @@
       </c>
       <c r="G19">
         <v>15</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
       </c>
       <c r="R19">
         <v>1</v>
@@ -2325,11 +2353,8 @@
         <v>52</v>
       </c>
       <c r="Z19" s="2"/>
-      <c r="AA19" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27">
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>68</v>
       </c>
@@ -2368,11 +2393,8 @@
         <v>55</v>
       </c>
       <c r="Z20" s="2"/>
-      <c r="AA20" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27">
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>72</v>
       </c>
@@ -2408,11 +2430,8 @@
         <v>58</v>
       </c>
       <c r="Z21" s="2"/>
-      <c r="AA21" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27">
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -2432,6 +2451,9 @@
         <v>1</v>
       </c>
       <c r="L22" s="3">
+        <v>1</v>
+      </c>
+      <c r="N22">
         <v>1</v>
       </c>
       <c r="Q22">
@@ -2445,11 +2467,8 @@
         <v>61</v>
       </c>
       <c r="Z22" s="2"/>
-      <c r="AA22" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27">
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -2464,6 +2483,12 @@
       </c>
       <c r="G23">
         <v>19.95</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
       </c>
       <c r="S23">
         <v>1</v>
@@ -2476,11 +2501,8 @@
         <v>64</v>
       </c>
       <c r="Z23" s="2"/>
-      <c r="AA23" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="24" spans="1:27">
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -2498,6 +2520,15 @@
       </c>
       <c r="G24">
         <v>19</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
       </c>
       <c r="R24">
         <v>1</v>
@@ -2522,11 +2553,8 @@
         <v>67</v>
       </c>
       <c r="Z24" s="2"/>
-      <c r="AA24" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27">
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>82</v>
       </c>
@@ -2546,9 +2574,6 @@
         <v>1</v>
       </c>
       <c r="O25">
-        <v>1</v>
-      </c>
-      <c r="P25">
         <v>1</v>
       </c>
       <c r="R25">
@@ -2568,11 +2593,8 @@
         <v>70</v>
       </c>
       <c r="Z25" s="2"/>
-      <c r="AA25" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27">
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>85</v>
       </c>
@@ -2608,11 +2630,8 @@
         <v>73</v>
       </c>
       <c r="Z26" s="2"/>
-      <c r="AA26" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27">
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>89</v>
       </c>
@@ -2651,11 +2670,8 @@
         <v>76</v>
       </c>
       <c r="Z27" s="2"/>
-      <c r="AA27" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="28" spans="1:27">
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>92</v>
       </c>
@@ -2670,6 +2686,15 @@
       </c>
       <c r="G28">
         <v>9.9499999999999993</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="P28">
+        <v>1</v>
       </c>
       <c r="R28">
         <v>1</v>
@@ -2688,11 +2713,8 @@
         <v>79</v>
       </c>
       <c r="Z28" s="2"/>
-      <c r="AA28" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="29" spans="1:27">
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>94</v>
       </c>
@@ -2713,6 +2735,15 @@
       </c>
       <c r="I29" t="s">
         <v>47</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="O29">
+        <v>1</v>
+      </c>
+      <c r="P29">
+        <v>1</v>
       </c>
       <c r="R29">
         <v>1</v>
@@ -2731,11 +2762,8 @@
         <v>82</v>
       </c>
       <c r="Z29" s="2"/>
-      <c r="AA29" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27" s="2" customFormat="1">
+    </row>
+    <row r="30" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>98</v>
       </c>
@@ -2756,6 +2784,15 @@
       </c>
       <c r="L30" s="3"/>
       <c r="M30" s="4"/>
+      <c r="N30" s="2">
+        <v>1</v>
+      </c>
+      <c r="O30" s="2">
+        <v>1</v>
+      </c>
+      <c r="P30" s="2">
+        <v>1</v>
+      </c>
       <c r="R30" s="2">
         <v>1</v>
       </c>
@@ -2772,11 +2809,8 @@
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="AA30" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="31" spans="1:27">
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>100</v>
       </c>
@@ -2794,6 +2828,21 @@
       </c>
       <c r="G31">
         <v>25</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
+      <c r="O31">
+        <v>1</v>
+      </c>
+      <c r="R31" s="2">
+        <v>1</v>
+      </c>
+      <c r="S31" s="2">
+        <v>1</v>
+      </c>
+      <c r="T31" s="2">
+        <v>1</v>
       </c>
       <c r="X31" s="2" t="s">
         <v>81</v>
@@ -2803,11 +2852,9 @@
         <v>88</v>
       </c>
       <c r="Z31" s="2"/>
-      <c r="AA31" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="32" spans="1:27">
+      <c r="AA31" s="2"/>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>103</v>
       </c>
@@ -2840,11 +2887,9 @@
         <v>91</v>
       </c>
       <c r="Z32" s="2"/>
-      <c r="AA32" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="33" spans="1:27">
+      <c r="AA32" s="2"/>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>107</v>
       </c>
@@ -2877,11 +2922,9 @@
         <v>94</v>
       </c>
       <c r="Z33" s="2"/>
-      <c r="AA33" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="34" spans="1:27">
+      <c r="AA33" s="2"/>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>110</v>
       </c>
@@ -2914,11 +2957,9 @@
         <v>97</v>
       </c>
       <c r="Z34" s="2"/>
-      <c r="AA34" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="35" spans="1:27">
+      <c r="AA34" s="2"/>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>113</v>
       </c>
@@ -2951,11 +2992,9 @@
         <v>100</v>
       </c>
       <c r="Z35" s="2"/>
-      <c r="AA35" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="36" spans="1:27">
+      <c r="AA35" s="2"/>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>115</v>
       </c>
@@ -2982,11 +3021,9 @@
         <v>103</v>
       </c>
       <c r="Z36" s="2"/>
-      <c r="AA36" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="37" spans="1:27">
+      <c r="AA36" s="2"/>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>118</v>
       </c>
@@ -3016,11 +3053,9 @@
         <v>106</v>
       </c>
       <c r="Z37" s="2"/>
-      <c r="AA37" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="38" spans="1:27">
+      <c r="AA37" s="2"/>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>122</v>
       </c>
@@ -3050,11 +3085,9 @@
         <v>109</v>
       </c>
       <c r="Z38" s="2"/>
-      <c r="AA38" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="39" spans="1:27">
+      <c r="AA38" s="2"/>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>125</v>
       </c>
@@ -3084,11 +3117,9 @@
         <v>112</v>
       </c>
       <c r="Z39" s="2"/>
-      <c r="AA39" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="40" spans="1:27" s="1" customFormat="1">
+      <c r="AA39" s="2"/>
+    </row>
+    <row r="40" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>128</v>
       </c>
@@ -3108,11 +3139,9 @@
         <v>115</v>
       </c>
       <c r="Z40" s="2"/>
-      <c r="AA40" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="41" spans="1:27">
+      <c r="AA40" s="2"/>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>129</v>
       </c>
@@ -3145,11 +3174,9 @@
         <v>118</v>
       </c>
       <c r="Z41" s="2"/>
-      <c r="AA41" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="42" spans="1:27">
+      <c r="AA41" s="2"/>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>133</v>
       </c>
@@ -3179,11 +3206,9 @@
         <v>121</v>
       </c>
       <c r="Z42" s="2"/>
-      <c r="AA42" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="43" spans="1:27">
+      <c r="AA42" s="2"/>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>136</v>
       </c>
@@ -3219,11 +3244,8 @@
         <v>124</v>
       </c>
       <c r="Z43" s="2"/>
-      <c r="AA43" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="44" spans="1:27">
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>139</v>
       </c>
@@ -3256,11 +3278,8 @@
         <v>127</v>
       </c>
       <c r="Z44" s="2"/>
-      <c r="AA44" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="45" spans="1:27">
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>141</v>
       </c>
@@ -3287,11 +3306,8 @@
         <v>130</v>
       </c>
       <c r="Z45" s="2"/>
-      <c r="AA45" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="46" spans="1:27">
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>143</v>
       </c>
@@ -3324,11 +3340,8 @@
         <v>133</v>
       </c>
       <c r="Z46" s="2"/>
-      <c r="AA46" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="47" spans="1:27">
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>146</v>
       </c>
@@ -3364,11 +3377,8 @@
         <v>136</v>
       </c>
       <c r="Z47" s="2"/>
-      <c r="AA47" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="48" spans="1:27" s="1" customFormat="1">
+    </row>
+    <row r="48" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>148</v>
       </c>
@@ -3385,11 +3395,9 @@
         <v>139</v>
       </c>
       <c r="Z48" s="2"/>
-      <c r="AA48" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="49" spans="1:27" s="1" customFormat="1">
+      <c r="AA48"/>
+    </row>
+    <row r="49" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>149</v>
       </c>
@@ -3406,11 +3414,9 @@
         <v>142</v>
       </c>
       <c r="Z49" s="2"/>
-      <c r="AA49" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="50" spans="1:27">
+      <c r="AA49"/>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>150</v>
       </c>
@@ -3444,7 +3450,7 @@
       </c>
       <c r="Z50" s="2"/>
     </row>
-    <row r="51" spans="1:27">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>154</v>
       </c>
@@ -3478,7 +3484,7 @@
       </c>
       <c r="Z51" s="2"/>
     </row>
-    <row r="52" spans="1:27">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>155</v>
       </c>
@@ -3512,7 +3518,7 @@
       </c>
       <c r="Z52" s="2"/>
     </row>
-    <row r="53" spans="1:27">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>159</v>
       </c>
@@ -3546,7 +3552,7 @@
       </c>
       <c r="Z53" s="2"/>
     </row>
-    <row r="54" spans="1:27">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>160</v>
       </c>
@@ -3580,7 +3586,7 @@
       </c>
       <c r="Z54" s="2"/>
     </row>
-    <row r="55" spans="1:27">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>161</v>
       </c>
@@ -3614,7 +3620,7 @@
       </c>
       <c r="Z55" s="2"/>
     </row>
-    <row r="56" spans="1:27">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>162</v>
       </c>
@@ -3648,7 +3654,7 @@
       </c>
       <c r="Z56" s="2"/>
     </row>
-    <row r="57" spans="1:27">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>164</v>
       </c>
@@ -3682,7 +3688,7 @@
       </c>
       <c r="Z57" s="2"/>
     </row>
-    <row r="58" spans="1:27">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>165</v>
       </c>
@@ -3716,7 +3722,7 @@
       </c>
       <c r="Z58" s="2"/>
     </row>
-    <row r="59" spans="1:27">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>167</v>
       </c>
@@ -3750,7 +3756,7 @@
       </c>
       <c r="Z59" s="2"/>
     </row>
-    <row r="60" spans="1:27">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>168</v>
       </c>
@@ -3784,7 +3790,7 @@
       </c>
       <c r="Z60" s="2"/>
     </row>
-    <row r="61" spans="1:27">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>169</v>
       </c>
@@ -3818,7 +3824,7 @@
       </c>
       <c r="Z61" s="2"/>
     </row>
-    <row r="62" spans="1:27">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>170</v>
       </c>
@@ -3852,7 +3858,7 @@
       </c>
       <c r="Z62" s="2"/>
     </row>
-    <row r="63" spans="1:27">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>171</v>
       </c>
@@ -3886,7 +3892,7 @@
       </c>
       <c r="Z63" s="2"/>
     </row>
-    <row r="64" spans="1:27">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>172</v>
       </c>
@@ -3920,7 +3926,7 @@
       </c>
       <c r="Z64" s="2"/>
     </row>
-    <row r="65" spans="1:26">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>173</v>
       </c>
@@ -3954,7 +3960,7 @@
       </c>
       <c r="Z65" s="2"/>
     </row>
-    <row r="66" spans="1:26">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>174</v>
       </c>
@@ -3988,7 +3994,7 @@
       </c>
       <c r="Z66" s="2"/>
     </row>
-    <row r="67" spans="1:26">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>175</v>
       </c>
@@ -4022,7 +4028,7 @@
       </c>
       <c r="Z67" s="2"/>
     </row>
-    <row r="68" spans="1:26">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>176</v>
       </c>
@@ -4056,7 +4062,7 @@
       </c>
       <c r="Z68" s="2"/>
     </row>
-    <row r="69" spans="1:26">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>177</v>
       </c>
@@ -4090,7 +4096,7 @@
       </c>
       <c r="Z69" s="2"/>
     </row>
-    <row r="70" spans="1:26">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>178</v>
       </c>
@@ -4124,7 +4130,7 @@
       </c>
       <c r="Z70" s="2"/>
     </row>
-    <row r="71" spans="1:26">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>179</v>
       </c>
@@ -4158,7 +4164,7 @@
       </c>
       <c r="Z71" s="2"/>
     </row>
-    <row r="72" spans="1:26">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>181</v>
       </c>
@@ -4178,6 +4184,9 @@
         <v>1</v>
       </c>
       <c r="O72">
+        <v>1</v>
+      </c>
+      <c r="Q72">
         <v>1</v>
       </c>
       <c r="R72">
@@ -4192,7 +4201,7 @@
       </c>
       <c r="Z72" s="2"/>
     </row>
-    <row r="73" spans="1:26">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>182</v>
       </c>
@@ -4212,6 +4221,9 @@
         <v>1</v>
       </c>
       <c r="O73">
+        <v>1</v>
+      </c>
+      <c r="Q73">
         <v>1</v>
       </c>
       <c r="R73">
@@ -4226,7 +4238,7 @@
       </c>
       <c r="Z73" s="2"/>
     </row>
-    <row r="74" spans="1:26">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>183</v>
       </c>
@@ -4246,6 +4258,9 @@
         <v>1</v>
       </c>
       <c r="O74">
+        <v>1</v>
+      </c>
+      <c r="Q74">
         <v>1</v>
       </c>
       <c r="R74">
@@ -4260,7 +4275,7 @@
       </c>
       <c r="Z74" s="2"/>
     </row>
-    <row r="75" spans="1:26">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>184</v>
       </c>
@@ -4280,6 +4295,9 @@
         <v>1</v>
       </c>
       <c r="O75">
+        <v>1</v>
+      </c>
+      <c r="Q75">
         <v>1</v>
       </c>
       <c r="R75">
@@ -4294,7 +4312,7 @@
       </c>
       <c r="Z75" s="2"/>
     </row>
-    <row r="76" spans="1:26">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>186</v>
       </c>
@@ -4314,6 +4332,9 @@
         <v>1</v>
       </c>
       <c r="O76">
+        <v>1</v>
+      </c>
+      <c r="Q76">
         <v>1</v>
       </c>
       <c r="R76">
@@ -4328,7 +4349,7 @@
       </c>
       <c r="Z76" s="2"/>
     </row>
-    <row r="77" spans="1:26">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>187</v>
       </c>
@@ -4348,6 +4369,9 @@
         <v>1</v>
       </c>
       <c r="O77">
+        <v>1</v>
+      </c>
+      <c r="Q77">
         <v>1</v>
       </c>
       <c r="R77">
@@ -4362,7 +4386,7 @@
       </c>
       <c r="Z77" s="2"/>
     </row>
-    <row r="78" spans="1:26">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>188</v>
       </c>
@@ -4382,6 +4406,9 @@
         <v>1</v>
       </c>
       <c r="O78">
+        <v>1</v>
+      </c>
+      <c r="Q78">
         <v>1</v>
       </c>
       <c r="R78">
@@ -4396,7 +4423,7 @@
       </c>
       <c r="Z78" s="2"/>
     </row>
-    <row r="79" spans="1:26">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>189</v>
       </c>
@@ -4416,6 +4443,9 @@
         <v>1</v>
       </c>
       <c r="O79">
+        <v>1</v>
+      </c>
+      <c r="Q79">
         <v>1</v>
       </c>
       <c r="R79">
@@ -4430,7 +4460,7 @@
       </c>
       <c r="Z79" s="2"/>
     </row>
-    <row r="80" spans="1:26">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>191</v>
       </c>
@@ -4456,6 +4486,9 @@
         <v>1</v>
       </c>
       <c r="R80">
+        <v>1</v>
+      </c>
+      <c r="T80">
         <v>1</v>
       </c>
       <c r="X80" s="2" t="s">
@@ -4467,7 +4500,7 @@
       </c>
       <c r="Z80" s="2"/>
     </row>
-    <row r="81" spans="1:27">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>193</v>
       </c>
@@ -4493,6 +4526,9 @@
         <v>1</v>
       </c>
       <c r="R81">
+        <v>1</v>
+      </c>
+      <c r="T81">
         <v>1</v>
       </c>
       <c r="X81" s="2" t="s">
@@ -4504,7 +4540,7 @@
       </c>
       <c r="Z81" s="2"/>
     </row>
-    <row r="82" spans="1:27">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>195</v>
       </c>
@@ -4530,6 +4566,9 @@
         <v>1</v>
       </c>
       <c r="R82">
+        <v>1</v>
+      </c>
+      <c r="T82">
         <v>1</v>
       </c>
       <c r="X82" s="2" t="s">
@@ -4541,7 +4580,7 @@
       </c>
       <c r="Z82" s="2"/>
     </row>
-    <row r="83" spans="1:27">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>197</v>
       </c>
@@ -4564,6 +4603,9 @@
         <v>1</v>
       </c>
       <c r="R83">
+        <v>1</v>
+      </c>
+      <c r="T83">
         <v>1</v>
       </c>
       <c r="X83" s="2" t="s">
@@ -4575,7 +4617,7 @@
       </c>
       <c r="Z83" s="2"/>
     </row>
-    <row r="84" spans="1:27" s="1" customFormat="1">
+    <row r="84" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>198</v>
       </c>
@@ -4583,6 +4625,15 @@
         <v>1</v>
       </c>
       <c r="P84"/>
+      <c r="R84" s="1">
+        <v>1</v>
+      </c>
+      <c r="T84" s="1">
+        <v>1</v>
+      </c>
+      <c r="U84" s="1">
+        <v>1</v>
+      </c>
       <c r="X84" s="2" t="s">
         <v>190</v>
       </c>
@@ -4593,7 +4644,7 @@
       <c r="Z84" s="2"/>
       <c r="AA84"/>
     </row>
-    <row r="85" spans="1:27" s="1" customFormat="1">
+    <row r="85" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>199</v>
       </c>
@@ -4601,6 +4652,15 @@
         <v>1</v>
       </c>
       <c r="P85"/>
+      <c r="R85" s="1">
+        <v>1</v>
+      </c>
+      <c r="T85" s="1">
+        <v>1</v>
+      </c>
+      <c r="U85" s="1">
+        <v>1</v>
+      </c>
       <c r="X85" s="2" t="s">
         <v>190</v>
       </c>
@@ -4611,7 +4671,7 @@
       <c r="Z85" s="2"/>
       <c r="AA85"/>
     </row>
-    <row r="86" spans="1:27">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>200</v>
       </c>
@@ -4634,6 +4694,18 @@
         <v>1</v>
       </c>
       <c r="O86">
+        <v>1</v>
+      </c>
+      <c r="Q86">
+        <v>1</v>
+      </c>
+      <c r="R86">
+        <v>1</v>
+      </c>
+      <c r="T86">
+        <v>1</v>
+      </c>
+      <c r="U86">
         <v>1</v>
       </c>
       <c r="X86" s="2" t="s">
@@ -4645,7 +4717,7 @@
       </c>
       <c r="Z86" s="2"/>
     </row>
-    <row r="87" spans="1:27">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>203</v>
       </c>
@@ -4665,6 +4737,9 @@
         <v>39</v>
       </c>
       <c r="L87" s="3">
+        <v>1</v>
+      </c>
+      <c r="N87">
         <v>1</v>
       </c>
       <c r="R87">
@@ -4679,7 +4754,7 @@
       </c>
       <c r="Z87" s="2"/>
     </row>
-    <row r="88" spans="1:27">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>203</v>
       </c>
@@ -4699,6 +4774,9 @@
         <v>39</v>
       </c>
       <c r="L88" s="3">
+        <v>1</v>
+      </c>
+      <c r="O88">
         <v>1</v>
       </c>
       <c r="R88">
@@ -4713,7 +4791,7 @@
       </c>
       <c r="Z88" s="2"/>
     </row>
-    <row r="89" spans="1:27">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>205</v>
       </c>
@@ -4733,6 +4811,9 @@
         <v>79</v>
       </c>
       <c r="L89" s="3">
+        <v>1</v>
+      </c>
+      <c r="O89">
         <v>1</v>
       </c>
       <c r="R89">
@@ -4747,7 +4828,7 @@
       </c>
       <c r="Z89" s="2"/>
     </row>
-    <row r="90" spans="1:27">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>208</v>
       </c>
@@ -4767,6 +4848,9 @@
         <v>79</v>
       </c>
       <c r="L90" s="3">
+        <v>1</v>
+      </c>
+      <c r="O90">
         <v>1</v>
       </c>
       <c r="R90">
@@ -4781,7 +4865,7 @@
       </c>
       <c r="Z90" s="2"/>
     </row>
-    <row r="91" spans="1:27">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>209</v>
       </c>
@@ -4809,7 +4893,7 @@
       </c>
       <c r="Z91" s="2"/>
     </row>
-    <row r="92" spans="1:27">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>211</v>
       </c>
@@ -4824,6 +4908,21 @@
       </c>
       <c r="G92">
         <v>89</v>
+      </c>
+      <c r="N92">
+        <v>1</v>
+      </c>
+      <c r="O92">
+        <v>1</v>
+      </c>
+      <c r="R92">
+        <v>1</v>
+      </c>
+      <c r="S92">
+        <v>1</v>
+      </c>
+      <c r="T92">
+        <v>1</v>
       </c>
       <c r="X92" s="2" t="s">
         <v>204</v>
@@ -4834,7 +4933,7 @@
       </c>
       <c r="Z92" s="2"/>
     </row>
-    <row r="93" spans="1:27">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>212</v>
       </c>
@@ -4853,7 +4952,19 @@
       <c r="G93">
         <v>69</v>
       </c>
+      <c r="N93">
+        <v>1</v>
+      </c>
+      <c r="O93">
+        <v>1</v>
+      </c>
+      <c r="R93">
+        <v>1</v>
+      </c>
       <c r="S93">
+        <v>1</v>
+      </c>
+      <c r="T93">
         <v>1</v>
       </c>
       <c r="X93" s="2" t="s">
@@ -4865,7 +4976,7 @@
       </c>
       <c r="Z93" s="2"/>
     </row>
-    <row r="94" spans="1:27">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>214</v>
       </c>
@@ -4883,6 +4994,15 @@
       </c>
       <c r="G94">
         <v>5</v>
+      </c>
+      <c r="N94">
+        <v>1</v>
+      </c>
+      <c r="O94">
+        <v>1</v>
+      </c>
+      <c r="R94">
+        <v>1</v>
       </c>
       <c r="X94" s="2" t="s">
         <v>204</v>
@@ -4893,7 +5013,7 @@
       </c>
       <c r="Z94" s="2"/>
     </row>
-    <row r="95" spans="1:27">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>217</v>
       </c>
@@ -4911,6 +5031,21 @@
       </c>
       <c r="G95">
         <v>25</v>
+      </c>
+      <c r="N95">
+        <v>1</v>
+      </c>
+      <c r="O95">
+        <v>1</v>
+      </c>
+      <c r="R95">
+        <v>1</v>
+      </c>
+      <c r="S95">
+        <v>1</v>
+      </c>
+      <c r="T95">
+        <v>1</v>
       </c>
       <c r="X95" s="2" t="s">
         <v>204</v>
@@ -4921,7 +5056,7 @@
       </c>
       <c r="Z95" s="2"/>
     </row>
-    <row r="96" spans="1:27">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>220</v>
       </c>
@@ -4939,6 +5074,18 @@
       </c>
       <c r="G96">
         <v>119</v>
+      </c>
+      <c r="N96">
+        <v>1</v>
+      </c>
+      <c r="O96">
+        <v>1</v>
+      </c>
+      <c r="R96">
+        <v>1</v>
+      </c>
+      <c r="S96">
+        <v>1</v>
       </c>
       <c r="X96" s="2" t="s">
         <v>204</v>
@@ -4949,7 +5096,7 @@
       </c>
       <c r="Z96" s="2"/>
     </row>
-    <row r="97" spans="1:26">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>223</v>
       </c>
@@ -4967,6 +5114,24 @@
       </c>
       <c r="I97" t="s">
         <v>24</v>
+      </c>
+      <c r="N97">
+        <v>1</v>
+      </c>
+      <c r="O97">
+        <v>1</v>
+      </c>
+      <c r="P97">
+        <v>1</v>
+      </c>
+      <c r="R97">
+        <v>1</v>
+      </c>
+      <c r="S97">
+        <v>1</v>
+      </c>
+      <c r="T97">
+        <v>1</v>
       </c>
       <c r="X97" s="2" t="s">
         <v>204</v>
@@ -4977,7 +5142,7 @@
       </c>
       <c r="Z97" s="2"/>
     </row>
-    <row r="98" spans="1:26">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>226</v>
       </c>
@@ -4998,6 +5163,18 @@
       </c>
       <c r="I98" t="s">
         <v>229</v>
+      </c>
+      <c r="N98">
+        <v>1</v>
+      </c>
+      <c r="O98">
+        <v>1</v>
+      </c>
+      <c r="R98">
+        <v>1</v>
+      </c>
+      <c r="S98">
+        <v>1</v>
       </c>
       <c r="X98" s="2" t="s">
         <v>204</v>
@@ -5008,7 +5185,7 @@
       </c>
       <c r="Z98" s="2"/>
     </row>
-    <row r="99" spans="1:26">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>230</v>
       </c>
@@ -5026,6 +5203,18 @@
       </c>
       <c r="G99">
         <v>19</v>
+      </c>
+      <c r="N99">
+        <v>1</v>
+      </c>
+      <c r="O99">
+        <v>1</v>
+      </c>
+      <c r="P99">
+        <v>1</v>
+      </c>
+      <c r="S99">
+        <v>1</v>
       </c>
       <c r="W99">
         <v>1</v>
@@ -5039,7 +5228,7 @@
       </c>
       <c r="Z99" s="2"/>
     </row>
-    <row r="100" spans="1:26">
+    <row r="100" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>234</v>
       </c>
@@ -5057,6 +5246,12 @@
       </c>
       <c r="G100">
         <v>349</v>
+      </c>
+      <c r="N100">
+        <v>1</v>
+      </c>
+      <c r="O100">
+        <v>1</v>
       </c>
       <c r="W100">
         <v>1</v>
@@ -5070,7 +5265,7 @@
       </c>
       <c r="Z100" s="2"/>
     </row>
-    <row r="101" spans="1:26">
+    <row r="101" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>237</v>
       </c>
@@ -5088,6 +5283,15 @@
       </c>
       <c r="G101">
         <v>39</v>
+      </c>
+      <c r="N101">
+        <v>1</v>
+      </c>
+      <c r="O101">
+        <v>1</v>
+      </c>
+      <c r="S101">
+        <v>1</v>
       </c>
       <c r="W101">
         <v>1</v>
@@ -5101,7 +5305,7 @@
       </c>
       <c r="Z101" s="2"/>
     </row>
-    <row r="102" spans="1:26">
+    <row r="102" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>239</v>
       </c>
@@ -5116,6 +5320,15 @@
       </c>
       <c r="G102">
         <v>69.95</v>
+      </c>
+      <c r="N102">
+        <v>1</v>
+      </c>
+      <c r="O102">
+        <v>1</v>
+      </c>
+      <c r="S102">
+        <v>1</v>
       </c>
       <c r="W102">
         <v>1</v>
@@ -5129,7 +5342,7 @@
       </c>
       <c r="Z102" s="2"/>
     </row>
-    <row r="103" spans="1:26">
+    <row r="103" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>242</v>
       </c>
@@ -5144,6 +5357,9 @@
       </c>
       <c r="G103">
         <v>799</v>
+      </c>
+      <c r="O103">
+        <v>1</v>
       </c>
       <c r="W103">
         <v>1</v>
@@ -5157,7 +5373,7 @@
       </c>
       <c r="Z103" s="2"/>
     </row>
-    <row r="104" spans="1:26">
+    <row r="104" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>30</v>
       </c>
@@ -5172,6 +5388,12 @@
       </c>
       <c r="G104">
         <v>69.95</v>
+      </c>
+      <c r="N104">
+        <v>1</v>
+      </c>
+      <c r="S104">
+        <v>1</v>
       </c>
       <c r="W104">
         <v>1</v>
@@ -5185,7 +5407,7 @@
       </c>
       <c r="Z104" s="2"/>
     </row>
-    <row r="105" spans="1:26">
+    <row r="105" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>247</v>
       </c>
@@ -5203,6 +5425,18 @@
       </c>
       <c r="I105" t="s">
         <v>121</v>
+      </c>
+      <c r="N105">
+        <v>1</v>
+      </c>
+      <c r="O105">
+        <v>1</v>
+      </c>
+      <c r="P105">
+        <v>1</v>
+      </c>
+      <c r="S105">
+        <v>1</v>
       </c>
       <c r="W105">
         <v>1</v>
@@ -5216,7 +5450,7 @@
       </c>
       <c r="Z105" s="2"/>
     </row>
-    <row r="106" spans="1:26">
+    <row r="106" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>250</v>
       </c>
@@ -5231,6 +5465,9 @@
       </c>
       <c r="G106">
         <v>599</v>
+      </c>
+      <c r="N106">
+        <v>1</v>
       </c>
       <c r="W106">
         <v>1</v>
@@ -5244,7 +5481,7 @@
       </c>
       <c r="Z106" s="2"/>
     </row>
-    <row r="107" spans="1:26">
+    <row r="107" spans="1:26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>253</v>
       </c>
@@ -5275,7 +5512,7 @@
       </c>
       <c r="Z107" s="2"/>
     </row>
-    <row r="108" spans="1:26">
+    <row r="108" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>255</v>
       </c>
@@ -5293,6 +5530,18 @@
       </c>
       <c r="G108">
         <v>179</v>
+      </c>
+      <c r="N108">
+        <v>1</v>
+      </c>
+      <c r="R108">
+        <v>1</v>
+      </c>
+      <c r="S108">
+        <v>1</v>
+      </c>
+      <c r="T108">
+        <v>1</v>
       </c>
       <c r="X108" t="s">
         <v>259</v>
@@ -5303,7 +5552,7 @@
       </c>
       <c r="Z108" s="2"/>
     </row>
-    <row r="109" spans="1:26">
+    <row r="109" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>256</v>
       </c>
@@ -5321,6 +5570,18 @@
       </c>
       <c r="G109">
         <v>175</v>
+      </c>
+      <c r="N109">
+        <v>1</v>
+      </c>
+      <c r="R109">
+        <v>1</v>
+      </c>
+      <c r="S109">
+        <v>1</v>
+      </c>
+      <c r="T109">
+        <v>1</v>
       </c>
       <c r="X109" t="s">
         <v>259</v>
@@ -5331,7 +5592,7 @@
       </c>
       <c r="Z109" s="2"/>
     </row>
-    <row r="110" spans="1:26">
+    <row r="110" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>260</v>
       </c>
@@ -5349,6 +5610,24 @@
       </c>
       <c r="I110" t="s">
         <v>280</v>
+      </c>
+      <c r="N110">
+        <v>1</v>
+      </c>
+      <c r="O110">
+        <v>1</v>
+      </c>
+      <c r="P110">
+        <v>1</v>
+      </c>
+      <c r="R110">
+        <v>1</v>
+      </c>
+      <c r="S110">
+        <v>1</v>
+      </c>
+      <c r="T110">
+        <v>1</v>
       </c>
       <c r="X110" t="s">
         <v>259</v>
@@ -5359,7 +5638,7 @@
       </c>
       <c r="Z110" s="2"/>
     </row>
-    <row r="111" spans="1:26">
+    <row r="111" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>261</v>
       </c>
@@ -5377,6 +5656,24 @@
       </c>
       <c r="I111" t="s">
         <v>281</v>
+      </c>
+      <c r="N111">
+        <v>1</v>
+      </c>
+      <c r="O111">
+        <v>1</v>
+      </c>
+      <c r="P111">
+        <v>1</v>
+      </c>
+      <c r="R111">
+        <v>1</v>
+      </c>
+      <c r="S111">
+        <v>1</v>
+      </c>
+      <c r="T111">
+        <v>1</v>
       </c>
       <c r="X111" t="s">
         <v>259</v>
@@ -5387,7 +5684,7 @@
       </c>
       <c r="Z111" s="2"/>
     </row>
-    <row r="112" spans="1:26">
+    <row r="112" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>262</v>
       </c>
@@ -5402,6 +5699,9 @@
       </c>
       <c r="G112">
         <v>399</v>
+      </c>
+      <c r="N112">
+        <v>1</v>
       </c>
       <c r="X112" t="s">
         <v>259</v>
@@ -5411,7 +5711,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="113" spans="1:25">
+    <row r="113" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>266</v>
       </c>
@@ -5429,6 +5729,21 @@
       </c>
       <c r="G113">
         <v>45</v>
+      </c>
+      <c r="N113">
+        <v>1</v>
+      </c>
+      <c r="O113">
+        <v>1</v>
+      </c>
+      <c r="R113">
+        <v>1</v>
+      </c>
+      <c r="S113">
+        <v>1</v>
+      </c>
+      <c r="T113">
+        <v>1</v>
       </c>
       <c r="X113" t="s">
         <v>259</v>
@@ -5438,7 +5753,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="114" spans="1:25">
+    <row r="114" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>265</v>
       </c>
@@ -5456,6 +5771,21 @@
       </c>
       <c r="G114">
         <v>19</v>
+      </c>
+      <c r="N114">
+        <v>1</v>
+      </c>
+      <c r="O114">
+        <v>1</v>
+      </c>
+      <c r="P114">
+        <v>1</v>
+      </c>
+      <c r="S114">
+        <v>1</v>
+      </c>
+      <c r="T114">
+        <v>1</v>
       </c>
       <c r="X114" t="s">
         <v>259</v>
@@ -5465,7 +5795,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="115" spans="1:25">
+    <row r="115" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>268</v>
       </c>
@@ -5477,6 +5807,21 @@
       </c>
       <c r="G115">
         <v>19.95</v>
+      </c>
+      <c r="N115">
+        <v>1</v>
+      </c>
+      <c r="O115">
+        <v>1</v>
+      </c>
+      <c r="P115">
+        <v>1</v>
+      </c>
+      <c r="S115">
+        <v>1</v>
+      </c>
+      <c r="T115">
+        <v>1</v>
       </c>
       <c r="X115" t="s">
         <v>259</v>
@@ -5486,7 +5831,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="116" spans="1:25">
+    <row r="116" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>270</v>
       </c>
@@ -5504,6 +5849,21 @@
       </c>
       <c r="G116">
         <v>69</v>
+      </c>
+      <c r="N116">
+        <v>1</v>
+      </c>
+      <c r="O116">
+        <v>1</v>
+      </c>
+      <c r="R116">
+        <v>1</v>
+      </c>
+      <c r="S116">
+        <v>1</v>
+      </c>
+      <c r="T116">
+        <v>1</v>
       </c>
       <c r="X116" t="s">
         <v>259</v>
@@ -5511,6 +5871,9 @@
       <c r="Y116" s="2">
         <f t="shared" si="3"/>
         <v>343</v>
+      </c>
+      <c r="Z116" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added placement numbers for filter pages
</commit_message>
<xml_diff>
--- a/excel/producten.xlsx
+++ b/excel/producten.xlsx
@@ -1668,8 +1668,8 @@
   <dimension ref="A1:AA117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F61" sqref="F61"/>
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1798,15 +1798,20 @@
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="4"/>
-      <c r="O2" s="2">
+      <c r="N2"/>
+      <c r="O2">
         <v>1</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="P2"/>
+      <c r="Q2">
         <v>1</v>
       </c>
-      <c r="R2" s="2">
-        <v>1</v>
-      </c>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
       <c r="X2" s="2" t="s">
         <v>29</v>
       </c>
@@ -1837,13 +1842,10 @@
         <v>24</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Q3">
-        <v>1</v>
-      </c>
-      <c r="R3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="X3" s="2" t="s">
         <v>29</v>
@@ -1883,13 +1885,10 @@
         <v>1</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="Q4">
-        <v>1</v>
-      </c>
-      <c r="R4">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="X4" s="2" t="s">
         <v>29</v>
@@ -1926,13 +1925,10 @@
         <v>1</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q5">
-        <v>1</v>
-      </c>
-      <c r="R5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="X5" s="2" t="s">
         <v>29</v>
@@ -1963,13 +1959,19 @@
         <v>19</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="R6">
+        <v>13</v>
       </c>
       <c r="S6">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="U6">
+        <v>13</v>
       </c>
       <c r="X6" s="2" t="s">
         <v>29</v>
@@ -1997,16 +1999,19 @@
         <v>29.95</v>
       </c>
       <c r="N7">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="O7">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="R7">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="S7">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="U7">
+        <v>16</v>
       </c>
       <c r="X7" s="2" t="s">
         <v>29</v>
@@ -2034,16 +2039,16 @@
         <v>44.95</v>
       </c>
       <c r="N8">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="O8">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="R8">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="S8">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="X8" s="2" t="s">
         <v>29</v>
@@ -2074,19 +2079,19 @@
         <v>43</v>
       </c>
       <c r="N9">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="O9">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="R9">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="S9">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="T9">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="X9" s="2" t="s">
         <v>29</v>
@@ -2120,19 +2125,19 @@
         <v>47</v>
       </c>
       <c r="N10">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="O10">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="R10">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="S10">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="T10">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="X10" s="2" t="s">
         <v>29</v>
@@ -2158,17 +2163,23 @@
       </c>
       <c r="L11" s="3"/>
       <c r="M11" s="4"/>
-      <c r="N11" s="1">
-        <v>1</v>
-      </c>
-      <c r="O11" s="1">
-        <v>1</v>
-      </c>
-      <c r="R11" s="1">
-        <v>1</v>
-      </c>
-      <c r="W11" s="1">
-        <v>1</v>
+      <c r="N11">
+        <v>28</v>
+      </c>
+      <c r="O11">
+        <v>28</v>
+      </c>
+      <c r="P11"/>
+      <c r="Q11"/>
+      <c r="R11">
+        <v>28</v>
+      </c>
+      <c r="S11"/>
+      <c r="T11"/>
+      <c r="U11"/>
+      <c r="V11"/>
+      <c r="W11">
+        <v>28</v>
       </c>
       <c r="X11" s="2" t="s">
         <v>29</v>
@@ -2205,10 +2216,10 @@
         <v>1</v>
       </c>
       <c r="O12">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="R12">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="X12" s="2" t="s">
         <v>71</v>
@@ -2242,19 +2253,19 @@
         <v>388</v>
       </c>
       <c r="N13">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="O13">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="R13">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="S13">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="T13">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="X13" s="2" t="s">
         <v>71</v>
@@ -2288,19 +2299,19 @@
         <v>389</v>
       </c>
       <c r="N14">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="O14">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="R14">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="S14">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="T14">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="X14" s="2" t="s">
         <v>71</v>
@@ -2334,13 +2345,16 @@
         <v>390</v>
       </c>
       <c r="N15">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="O15">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="S15">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="T15">
+        <v>40</v>
       </c>
       <c r="X15" s="2" t="s">
         <v>71</v>
@@ -2374,13 +2388,16 @@
         <v>390</v>
       </c>
       <c r="N16">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="O16">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="S16">
-        <v>1</v>
+        <v>43</v>
+      </c>
+      <c r="T16">
+        <v>43</v>
       </c>
       <c r="X16" s="2" t="s">
         <v>71</v>
@@ -2414,13 +2431,16 @@
         <v>390</v>
       </c>
       <c r="N17">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="O17">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="S17">
-        <v>1</v>
+        <v>46</v>
+      </c>
+      <c r="T17">
+        <v>46</v>
       </c>
       <c r="X17" s="2" t="s">
         <v>71</v>
@@ -2454,13 +2474,16 @@
         <v>43</v>
       </c>
       <c r="N18">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="O18">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="S18">
-        <v>1</v>
+        <v>49</v>
+      </c>
+      <c r="T18">
+        <v>49</v>
       </c>
       <c r="X18" s="2" t="s">
         <v>71</v>
@@ -2491,19 +2514,19 @@
         <v>15</v>
       </c>
       <c r="N19">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="O19">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="R19">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="S19">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="T19">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="X19" s="2" t="s">
         <v>71</v>
@@ -2543,10 +2566,13 @@
         <v>1</v>
       </c>
       <c r="N20">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="Q20">
-        <v>1</v>
+        <v>55</v>
+      </c>
+      <c r="U20">
+        <v>55</v>
       </c>
       <c r="X20" s="2" t="s">
         <v>71</v>
@@ -2586,10 +2612,13 @@
         <v>1</v>
       </c>
       <c r="N21">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="Q21">
-        <v>1</v>
+        <v>58</v>
+      </c>
+      <c r="U21">
+        <v>58</v>
       </c>
       <c r="X21" s="2" t="s">
         <v>71</v>
@@ -2626,10 +2655,10 @@
         <v>1</v>
       </c>
       <c r="N22">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="Q22">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="X22" s="2" t="s">
         <v>71</v>
@@ -2657,13 +2686,13 @@
         <v>19.95</v>
       </c>
       <c r="N23">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="O23">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="S23">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="X23" s="2" t="s">
         <v>71</v>
@@ -2697,28 +2726,28 @@
         <v>394</v>
       </c>
       <c r="N24">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="O24">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="P24">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="R24">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="S24">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="T24">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="U24">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="V24">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="X24" s="2" t="s">
         <v>81</v>
@@ -2749,19 +2778,19 @@
         <v>395</v>
       </c>
       <c r="N25">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="O25">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="R25">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="S25">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="T25">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="X25" s="2" t="s">
         <v>81</v>
@@ -2789,16 +2818,16 @@
         <v>49.95</v>
       </c>
       <c r="P26">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="R26">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="S26">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="T26">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="X26" s="2" t="s">
         <v>81</v>
@@ -2832,16 +2861,16 @@
         <v>278</v>
       </c>
       <c r="P27">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="R27">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="S27">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="T27">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="X27" s="2" t="s">
         <v>81</v>
@@ -2869,22 +2898,25 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="N28">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="O28">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="P28">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="R28">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="S28">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="T28">
-        <v>1</v>
+        <v>79</v>
+      </c>
+      <c r="U28">
+        <v>79</v>
       </c>
       <c r="X28" s="2" t="s">
         <v>81</v>
@@ -2918,22 +2950,22 @@
         <v>47</v>
       </c>
       <c r="N29">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="O29">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="P29">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="R29">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="S29">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="T29">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="X29" s="2" t="s">
         <v>81</v>
@@ -2965,24 +2997,28 @@
       </c>
       <c r="L30" s="3"/>
       <c r="M30" s="4"/>
-      <c r="N30" s="2">
-        <v>1</v>
-      </c>
-      <c r="O30" s="2">
-        <v>1</v>
-      </c>
-      <c r="P30" s="2">
-        <v>1</v>
-      </c>
-      <c r="R30" s="2">
-        <v>1</v>
-      </c>
-      <c r="S30" s="2">
-        <v>1</v>
-      </c>
-      <c r="T30" s="2">
-        <v>1</v>
-      </c>
+      <c r="N30">
+        <v>85</v>
+      </c>
+      <c r="O30">
+        <v>85</v>
+      </c>
+      <c r="P30">
+        <v>85</v>
+      </c>
+      <c r="Q30"/>
+      <c r="R30">
+        <v>85</v>
+      </c>
+      <c r="S30">
+        <v>85</v>
+      </c>
+      <c r="T30">
+        <v>85</v>
+      </c>
+      <c r="U30"/>
+      <c r="V30"/>
+      <c r="W30"/>
       <c r="X30" s="2" t="s">
         <v>81</v>
       </c>
@@ -3011,19 +3047,19 @@
         <v>25</v>
       </c>
       <c r="N31">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="O31">
-        <v>1</v>
-      </c>
-      <c r="R31" s="2">
-        <v>1</v>
-      </c>
-      <c r="S31" s="2">
-        <v>1</v>
-      </c>
-      <c r="T31" s="2">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="R31">
+        <v>88</v>
+      </c>
+      <c r="S31">
+        <v>88</v>
+      </c>
+      <c r="T31">
+        <v>88</v>
       </c>
       <c r="X31" s="2" t="s">
         <v>81</v>
@@ -3058,10 +3094,10 @@
         <v>1</v>
       </c>
       <c r="P32">
-        <v>1</v>
+        <v>91</v>
       </c>
       <c r="V32">
-        <v>1</v>
+        <v>91</v>
       </c>
       <c r="X32" s="2" t="s">
         <v>105</v>
@@ -3096,10 +3132,10 @@
         <v>1</v>
       </c>
       <c r="P33">
-        <v>1</v>
+        <v>94</v>
       </c>
       <c r="V33">
-        <v>1</v>
+        <v>94</v>
       </c>
       <c r="X33" s="2" t="s">
         <v>105</v>
@@ -3134,10 +3170,10 @@
         <v>1</v>
       </c>
       <c r="P34">
-        <v>1</v>
+        <v>97</v>
       </c>
       <c r="V34">
-        <v>1</v>
+        <v>97</v>
       </c>
       <c r="X34" s="2" t="s">
         <v>105</v>
@@ -3172,10 +3208,10 @@
         <v>1</v>
       </c>
       <c r="P35">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="V35">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="X35" s="2" t="s">
         <v>105</v>
@@ -3210,10 +3246,10 @@
         <v>1</v>
       </c>
       <c r="P36">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="V36">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="X36" s="2" t="s">
         <v>105</v>
@@ -3245,10 +3281,13 @@
         <v>397</v>
       </c>
       <c r="P37">
-        <v>1</v>
+        <v>106</v>
+      </c>
+      <c r="Q37">
+        <v>106</v>
       </c>
       <c r="V37">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="X37" s="2" t="s">
         <v>105</v>
@@ -3277,10 +3316,13 @@
         <v>120</v>
       </c>
       <c r="P38">
-        <v>1</v>
+        <v>109</v>
+      </c>
+      <c r="Q38">
+        <v>109</v>
       </c>
       <c r="V38">
-        <v>1</v>
+        <v>109</v>
       </c>
       <c r="X38" s="2" t="s">
         <v>105</v>
@@ -3309,10 +3351,10 @@
         <v>15</v>
       </c>
       <c r="P39">
-        <v>1</v>
+        <v>112</v>
       </c>
       <c r="V39">
-        <v>1</v>
+        <v>112</v>
       </c>
       <c r="X39" s="2" t="s">
         <v>105</v>
@@ -3341,10 +3383,10 @@
         <v>120</v>
       </c>
       <c r="P40">
-        <v>1</v>
+        <v>115</v>
       </c>
       <c r="V40">
-        <v>1</v>
+        <v>115</v>
       </c>
       <c r="X40" s="2" t="s">
         <v>105</v>
@@ -3362,12 +3404,24 @@
       </c>
       <c r="L41" s="3"/>
       <c r="M41" s="4"/>
-      <c r="P41" s="1">
-        <v>1</v>
-      </c>
-      <c r="V41" s="1">
-        <v>1</v>
-      </c>
+      <c r="N41"/>
+      <c r="O41"/>
+      <c r="P41">
+        <v>118</v>
+      </c>
+      <c r="Q41">
+        <v>118</v>
+      </c>
+      <c r="R41"/>
+      <c r="S41"/>
+      <c r="T41"/>
+      <c r="U41">
+        <v>118</v>
+      </c>
+      <c r="V41">
+        <v>118</v>
+      </c>
+      <c r="W41"/>
       <c r="X41" s="2" t="s">
         <v>105</v>
       </c>
@@ -3401,13 +3455,19 @@
         <v>1</v>
       </c>
       <c r="N42">
-        <v>1</v>
+        <v>121</v>
       </c>
       <c r="O42">
-        <v>1</v>
+        <v>121</v>
+      </c>
+      <c r="Q42">
+        <v>121</v>
+      </c>
+      <c r="R42">
+        <v>121</v>
       </c>
       <c r="U42">
-        <v>1</v>
+        <v>121</v>
       </c>
       <c r="X42" s="2" t="s">
         <v>131</v>
@@ -3439,7 +3499,7 @@
         <v>1</v>
       </c>
       <c r="U43">
-        <v>1</v>
+        <v>124</v>
       </c>
       <c r="X43" s="2" t="s">
         <v>131</v>
@@ -3477,10 +3537,13 @@
         <v>1</v>
       </c>
       <c r="O44">
-        <v>1</v>
+        <v>127</v>
+      </c>
+      <c r="Q44">
+        <v>127</v>
       </c>
       <c r="U44">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="X44" s="2" t="s">
         <v>131</v>
@@ -3514,10 +3577,10 @@
         <v>1</v>
       </c>
       <c r="N45">
-        <v>1</v>
+        <v>130</v>
       </c>
       <c r="U45">
-        <v>1</v>
+        <v>130</v>
       </c>
       <c r="X45" s="2" t="s">
         <v>131</v>
@@ -3550,8 +3613,11 @@
       <c r="I46" t="s">
         <v>24</v>
       </c>
+      <c r="N46">
+        <v>133</v>
+      </c>
       <c r="U46">
-        <v>1</v>
+        <v>133</v>
       </c>
       <c r="X46" s="2" t="s">
         <v>131</v>
@@ -3585,10 +3651,13 @@
         <v>1</v>
       </c>
       <c r="N47">
-        <v>1</v>
+        <v>136</v>
+      </c>
+      <c r="Q47">
+        <v>136</v>
       </c>
       <c r="U47">
-        <v>1</v>
+        <v>136</v>
       </c>
       <c r="X47" s="2" t="s">
         <v>131</v>
@@ -3622,10 +3691,10 @@
         <v>1</v>
       </c>
       <c r="O48">
-        <v>1</v>
+        <v>139</v>
       </c>
       <c r="U48">
-        <v>1</v>
+        <v>139</v>
       </c>
       <c r="X48" s="2" t="s">
         <v>131</v>
@@ -3642,9 +3711,18 @@
       </c>
       <c r="L49" s="3"/>
       <c r="M49" s="4"/>
-      <c r="U49" s="1">
-        <v>1</v>
-      </c>
+      <c r="N49"/>
+      <c r="O49"/>
+      <c r="P49"/>
+      <c r="Q49"/>
+      <c r="R49"/>
+      <c r="S49"/>
+      <c r="T49"/>
+      <c r="U49">
+        <v>142</v>
+      </c>
+      <c r="V49"/>
+      <c r="W49"/>
       <c r="X49" s="2" t="s">
         <v>131</v>
       </c>
@@ -3661,9 +3739,18 @@
       </c>
       <c r="L50" s="3"/>
       <c r="M50" s="4"/>
-      <c r="U50" s="1">
-        <v>1</v>
-      </c>
+      <c r="N50"/>
+      <c r="O50"/>
+      <c r="P50"/>
+      <c r="Q50"/>
+      <c r="R50"/>
+      <c r="S50"/>
+      <c r="T50"/>
+      <c r="U50">
+        <v>145</v>
+      </c>
+      <c r="V50"/>
+      <c r="W50"/>
       <c r="X50" s="2" t="s">
         <v>131</v>
       </c>
@@ -3694,10 +3781,10 @@
         <v>1</v>
       </c>
       <c r="N51">
-        <v>1</v>
+        <v>148</v>
       </c>
       <c r="R51">
-        <v>1</v>
+        <v>148</v>
       </c>
       <c r="X51" s="2" t="s">
         <v>152</v>
@@ -3728,10 +3815,7 @@
         <v>1</v>
       </c>
       <c r="N52">
-        <v>1</v>
-      </c>
-      <c r="R52">
-        <v>1</v>
+        <v>151</v>
       </c>
       <c r="X52" s="2" t="s">
         <v>152</v>
@@ -3765,10 +3849,7 @@
         <v>1</v>
       </c>
       <c r="N53">
-        <v>1</v>
-      </c>
-      <c r="R53">
-        <v>1</v>
+        <v>154</v>
       </c>
       <c r="X53" s="2" t="s">
         <v>152</v>
@@ -3802,10 +3883,7 @@
         <v>1</v>
       </c>
       <c r="N54">
-        <v>1</v>
-      </c>
-      <c r="R54">
-        <v>1</v>
+        <v>157</v>
       </c>
       <c r="X54" s="2" t="s">
         <v>152</v>
@@ -3839,10 +3917,7 @@
         <v>1</v>
       </c>
       <c r="N55">
-        <v>1</v>
-      </c>
-      <c r="R55">
-        <v>1</v>
+        <v>160</v>
       </c>
       <c r="X55" s="2" t="s">
         <v>152</v>
@@ -3876,10 +3951,7 @@
         <v>1</v>
       </c>
       <c r="N56">
-        <v>1</v>
-      </c>
-      <c r="R56">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="X56" s="2" t="s">
         <v>152</v>
@@ -3910,10 +3982,7 @@
         <v>1</v>
       </c>
       <c r="O57">
-        <v>1</v>
-      </c>
-      <c r="R57">
-        <v>1</v>
+        <v>166</v>
       </c>
       <c r="X57" s="2" t="s">
         <v>152</v>
@@ -3944,10 +4013,7 @@
         <v>1</v>
       </c>
       <c r="O58">
-        <v>1</v>
-      </c>
-      <c r="R58">
-        <v>1</v>
+        <v>169</v>
       </c>
       <c r="X58" s="2" t="s">
         <v>152</v>
@@ -3981,10 +4047,7 @@
         <v>1</v>
       </c>
       <c r="O59">
-        <v>1</v>
-      </c>
-      <c r="R59">
-        <v>1</v>
+        <v>172</v>
       </c>
       <c r="X59" s="2" t="s">
         <v>152</v>
@@ -4018,10 +4081,7 @@
         <v>1</v>
       </c>
       <c r="O60">
-        <v>1</v>
-      </c>
-      <c r="R60">
-        <v>1</v>
+        <v>175</v>
       </c>
       <c r="X60" s="2" t="s">
         <v>152</v>
@@ -4052,10 +4112,7 @@
         <v>1</v>
       </c>
       <c r="O61">
-        <v>1</v>
-      </c>
-      <c r="R61">
-        <v>1</v>
+        <v>178</v>
       </c>
       <c r="X61" s="2" t="s">
         <v>152</v>
@@ -4086,10 +4143,7 @@
         <v>1</v>
       </c>
       <c r="O62">
-        <v>1</v>
-      </c>
-      <c r="R62">
-        <v>1</v>
+        <v>181</v>
       </c>
       <c r="X62" s="2" t="s">
         <v>152</v>
@@ -4120,10 +4174,7 @@
         <v>1</v>
       </c>
       <c r="O63">
-        <v>1</v>
-      </c>
-      <c r="R63">
-        <v>1</v>
+        <v>184</v>
       </c>
       <c r="X63" s="2" t="s">
         <v>152</v>
@@ -4154,10 +4205,7 @@
         <v>1</v>
       </c>
       <c r="O64">
-        <v>1</v>
-      </c>
-      <c r="R64">
-        <v>1</v>
+        <v>187</v>
       </c>
       <c r="X64" s="2" t="s">
         <v>152</v>
@@ -4191,10 +4239,7 @@
         <v>1</v>
       </c>
       <c r="O65">
-        <v>1</v>
-      </c>
-      <c r="R65">
-        <v>1</v>
+        <v>190</v>
       </c>
       <c r="X65" s="2" t="s">
         <v>152</v>
@@ -4225,10 +4270,7 @@
         <v>1</v>
       </c>
       <c r="O66">
-        <v>1</v>
-      </c>
-      <c r="R66">
-        <v>1</v>
+        <v>193</v>
       </c>
       <c r="X66" s="2" t="s">
         <v>152</v>
@@ -4259,10 +4301,7 @@
         <v>1</v>
       </c>
       <c r="O67">
-        <v>1</v>
-      </c>
-      <c r="R67">
-        <v>1</v>
+        <v>196</v>
       </c>
       <c r="X67" s="2" t="s">
         <v>152</v>
@@ -4293,10 +4332,7 @@
         <v>1</v>
       </c>
       <c r="O68">
-        <v>1</v>
-      </c>
-      <c r="R68">
-        <v>1</v>
+        <v>199</v>
       </c>
       <c r="X68" s="2" t="s">
         <v>152</v>
@@ -4327,10 +4363,7 @@
         <v>1</v>
       </c>
       <c r="O69">
-        <v>1</v>
-      </c>
-      <c r="R69">
-        <v>1</v>
+        <v>202</v>
       </c>
       <c r="X69" s="2" t="s">
         <v>152</v>
@@ -4364,10 +4397,7 @@
         <v>1</v>
       </c>
       <c r="O70">
-        <v>1</v>
-      </c>
-      <c r="R70">
-        <v>1</v>
+        <v>205</v>
       </c>
       <c r="X70" s="2" t="s">
         <v>152</v>
@@ -4401,10 +4431,7 @@
         <v>1</v>
       </c>
       <c r="O71">
-        <v>1</v>
-      </c>
-      <c r="R71">
-        <v>1</v>
+        <v>208</v>
       </c>
       <c r="X71" s="2" t="s">
         <v>152</v>
@@ -4435,10 +4462,7 @@
         <v>1</v>
       </c>
       <c r="O72">
-        <v>1</v>
-      </c>
-      <c r="R72">
-        <v>1</v>
+        <v>211</v>
       </c>
       <c r="X72" s="2" t="s">
         <v>152</v>
@@ -4469,13 +4493,10 @@
         <v>1</v>
       </c>
       <c r="O73">
-        <v>1</v>
+        <v>214</v>
       </c>
       <c r="Q73">
-        <v>1</v>
-      </c>
-      <c r="R73">
-        <v>1</v>
+        <v>214</v>
       </c>
       <c r="X73" s="2" t="s">
         <v>152</v>
@@ -4506,13 +4527,10 @@
         <v>1</v>
       </c>
       <c r="O74">
-        <v>1</v>
+        <v>217</v>
       </c>
       <c r="Q74">
-        <v>1</v>
-      </c>
-      <c r="R74">
-        <v>1</v>
+        <v>217</v>
       </c>
       <c r="X74" s="2" t="s">
         <v>152</v>
@@ -4543,13 +4561,10 @@
         <v>1</v>
       </c>
       <c r="O75">
-        <v>1</v>
+        <v>220</v>
       </c>
       <c r="Q75">
-        <v>1</v>
-      </c>
-      <c r="R75">
-        <v>1</v>
+        <v>220</v>
       </c>
       <c r="X75" s="2" t="s">
         <v>152</v>
@@ -4580,13 +4595,10 @@
         <v>1</v>
       </c>
       <c r="O76">
-        <v>1</v>
+        <v>223</v>
       </c>
       <c r="Q76">
-        <v>1</v>
-      </c>
-      <c r="R76">
-        <v>1</v>
+        <v>223</v>
       </c>
       <c r="X76" s="2" t="s">
         <v>152</v>
@@ -4617,13 +4629,10 @@
         <v>1</v>
       </c>
       <c r="O77">
-        <v>1</v>
+        <v>226</v>
       </c>
       <c r="Q77">
-        <v>1</v>
-      </c>
-      <c r="R77">
-        <v>1</v>
+        <v>226</v>
       </c>
       <c r="X77" s="2" t="s">
         <v>152</v>
@@ -4654,13 +4663,10 @@
         <v>1</v>
       </c>
       <c r="O78">
-        <v>1</v>
+        <v>229</v>
       </c>
       <c r="Q78">
-        <v>1</v>
-      </c>
-      <c r="R78">
-        <v>1</v>
+        <v>229</v>
       </c>
       <c r="X78" s="2" t="s">
         <v>152</v>
@@ -4691,13 +4697,10 @@
         <v>1</v>
       </c>
       <c r="O79">
-        <v>1</v>
+        <v>232</v>
       </c>
       <c r="Q79">
-        <v>1</v>
-      </c>
-      <c r="R79">
-        <v>1</v>
+        <v>232</v>
       </c>
       <c r="X79" s="2" t="s">
         <v>152</v>
@@ -4728,13 +4731,10 @@
         <v>1</v>
       </c>
       <c r="O80">
-        <v>1</v>
+        <v>235</v>
       </c>
       <c r="Q80">
-        <v>1</v>
-      </c>
-      <c r="R80">
-        <v>1</v>
+        <v>235</v>
       </c>
       <c r="X80" s="2" t="s">
         <v>152</v>
@@ -4768,13 +4768,19 @@
         <v>1</v>
       </c>
       <c r="N81">
-        <v>1</v>
+        <v>238</v>
+      </c>
+      <c r="Q81">
+        <v>238</v>
       </c>
       <c r="R81">
-        <v>1</v>
+        <v>238</v>
       </c>
       <c r="T81">
-        <v>1</v>
+        <v>238</v>
+      </c>
+      <c r="U81">
+        <v>238</v>
       </c>
       <c r="X81" s="2" t="s">
         <v>189</v>
@@ -4808,13 +4814,19 @@
         <v>1</v>
       </c>
       <c r="N82">
-        <v>1</v>
+        <v>241</v>
+      </c>
+      <c r="Q82">
+        <v>241</v>
       </c>
       <c r="R82">
-        <v>1</v>
+        <v>241</v>
       </c>
       <c r="T82">
-        <v>1</v>
+        <v>241</v>
+      </c>
+      <c r="U82">
+        <v>241</v>
       </c>
       <c r="X82" s="2" t="s">
         <v>189</v>
@@ -4848,13 +4860,19 @@
         <v>1</v>
       </c>
       <c r="N83">
-        <v>1</v>
+        <v>244</v>
+      </c>
+      <c r="Q83">
+        <v>244</v>
       </c>
       <c r="R83">
-        <v>1</v>
+        <v>244</v>
       </c>
       <c r="T83">
-        <v>1</v>
+        <v>244</v>
+      </c>
+      <c r="U83">
+        <v>244</v>
       </c>
       <c r="X83" s="2" t="s">
         <v>189</v>
@@ -4885,13 +4903,19 @@
         <v>1</v>
       </c>
       <c r="N84">
-        <v>1</v>
+        <v>247</v>
+      </c>
+      <c r="Q84">
+        <v>247</v>
       </c>
       <c r="R84">
-        <v>1</v>
+        <v>247</v>
       </c>
       <c r="T84">
-        <v>1</v>
+        <v>247</v>
+      </c>
+      <c r="U84">
+        <v>247</v>
       </c>
       <c r="X84" s="2" t="s">
         <v>189</v>
@@ -4906,19 +4930,26 @@
       <c r="A85" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="N85" s="1">
-        <v>1</v>
-      </c>
+      <c r="N85">
+        <v>250</v>
+      </c>
+      <c r="O85"/>
       <c r="P85"/>
-      <c r="R85" s="1">
-        <v>1</v>
-      </c>
-      <c r="T85" s="1">
-        <v>1</v>
-      </c>
-      <c r="U85" s="1">
-        <v>1</v>
-      </c>
+      <c r="Q85">
+        <v>250</v>
+      </c>
+      <c r="R85">
+        <v>250</v>
+      </c>
+      <c r="S85"/>
+      <c r="T85">
+        <v>250</v>
+      </c>
+      <c r="U85">
+        <v>250</v>
+      </c>
+      <c r="V85"/>
+      <c r="W85"/>
       <c r="X85" s="2" t="s">
         <v>189</v>
       </c>
@@ -4933,19 +4964,26 @@
       <c r="A86" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="O86" s="1">
-        <v>1</v>
+      <c r="N86"/>
+      <c r="O86">
+        <v>253</v>
       </c>
       <c r="P86"/>
-      <c r="R86" s="1">
-        <v>1</v>
-      </c>
-      <c r="T86" s="1">
-        <v>1</v>
-      </c>
-      <c r="U86" s="1">
-        <v>1</v>
-      </c>
+      <c r="Q86">
+        <v>253</v>
+      </c>
+      <c r="R86">
+        <v>253</v>
+      </c>
+      <c r="S86"/>
+      <c r="T86">
+        <v>253</v>
+      </c>
+      <c r="U86">
+        <v>253</v>
+      </c>
+      <c r="V86"/>
+      <c r="W86"/>
       <c r="X86" s="2" t="s">
         <v>189</v>
       </c>
@@ -4976,22 +5014,22 @@
         <v>25</v>
       </c>
       <c r="N87">
-        <v>1</v>
+        <v>256</v>
       </c>
       <c r="O87">
-        <v>1</v>
+        <v>256</v>
       </c>
       <c r="Q87">
-        <v>1</v>
+        <v>256</v>
       </c>
       <c r="R87">
-        <v>1</v>
+        <v>256</v>
       </c>
       <c r="T87">
-        <v>1</v>
+        <v>256</v>
       </c>
       <c r="U87">
-        <v>1</v>
+        <v>256</v>
       </c>
       <c r="X87" s="2" t="s">
         <v>189</v>
@@ -5025,10 +5063,10 @@
         <v>1</v>
       </c>
       <c r="N88">
-        <v>1</v>
+        <v>259</v>
       </c>
       <c r="R88">
-        <v>1</v>
+        <v>259</v>
       </c>
       <c r="X88" s="2" t="s">
         <v>203</v>
@@ -5062,10 +5100,10 @@
         <v>1</v>
       </c>
       <c r="O89">
-        <v>1</v>
+        <v>262</v>
       </c>
       <c r="R89">
-        <v>1</v>
+        <v>262</v>
       </c>
       <c r="X89" s="2" t="s">
         <v>203</v>
@@ -5099,10 +5137,10 @@
         <v>1</v>
       </c>
       <c r="O90">
-        <v>1</v>
+        <v>265</v>
       </c>
       <c r="R90">
-        <v>1</v>
+        <v>265</v>
       </c>
       <c r="X90" s="2" t="s">
         <v>203</v>
@@ -5136,10 +5174,10 @@
         <v>1</v>
       </c>
       <c r="O91">
-        <v>1</v>
+        <v>268</v>
       </c>
       <c r="R91">
-        <v>1</v>
+        <v>268</v>
       </c>
       <c r="X91" s="2" t="s">
         <v>203</v>
@@ -5169,6 +5207,15 @@
       <c r="G92">
         <v>85</v>
       </c>
+      <c r="N92">
+        <v>271</v>
+      </c>
+      <c r="O92">
+        <v>271</v>
+      </c>
+      <c r="T92">
+        <v>271</v>
+      </c>
       <c r="X92" s="2" t="s">
         <v>203</v>
       </c>
@@ -5195,19 +5242,19 @@
         <v>89</v>
       </c>
       <c r="N93">
-        <v>1</v>
+        <v>274</v>
       </c>
       <c r="O93">
-        <v>1</v>
+        <v>274</v>
       </c>
       <c r="R93">
-        <v>1</v>
+        <v>274</v>
       </c>
       <c r="S93">
-        <v>1</v>
+        <v>274</v>
       </c>
       <c r="T93">
-        <v>1</v>
+        <v>274</v>
       </c>
       <c r="X93" s="2" t="s">
         <v>203</v>
@@ -5238,19 +5285,19 @@
         <v>69</v>
       </c>
       <c r="N94">
-        <v>1</v>
+        <v>277</v>
       </c>
       <c r="O94">
-        <v>1</v>
+        <v>277</v>
       </c>
       <c r="R94">
-        <v>1</v>
+        <v>277</v>
       </c>
       <c r="S94">
-        <v>1</v>
+        <v>277</v>
       </c>
       <c r="T94">
-        <v>1</v>
+        <v>277</v>
       </c>
       <c r="X94" s="2" t="s">
         <v>203</v>
@@ -5281,13 +5328,13 @@
         <v>5</v>
       </c>
       <c r="N95">
-        <v>1</v>
+        <v>280</v>
       </c>
       <c r="O95">
-        <v>1</v>
+        <v>280</v>
       </c>
       <c r="R95">
-        <v>1</v>
+        <v>280</v>
       </c>
       <c r="X95" s="2" t="s">
         <v>203</v>
@@ -5318,19 +5365,19 @@
         <v>25</v>
       </c>
       <c r="N96">
-        <v>1</v>
+        <v>283</v>
       </c>
       <c r="O96">
-        <v>1</v>
+        <v>283</v>
       </c>
       <c r="R96">
-        <v>1</v>
+        <v>283</v>
       </c>
       <c r="S96">
-        <v>1</v>
+        <v>283</v>
       </c>
       <c r="T96">
-        <v>1</v>
+        <v>283</v>
       </c>
       <c r="X96" s="2" t="s">
         <v>203</v>
@@ -5361,16 +5408,16 @@
         <v>119</v>
       </c>
       <c r="N97">
-        <v>1</v>
+        <v>286</v>
       </c>
       <c r="O97">
-        <v>1</v>
+        <v>286</v>
       </c>
       <c r="R97">
-        <v>1</v>
+        <v>286</v>
       </c>
       <c r="S97">
-        <v>1</v>
+        <v>286</v>
       </c>
       <c r="X97" s="2" t="s">
         <v>203</v>
@@ -5401,22 +5448,22 @@
         <v>24</v>
       </c>
       <c r="N98">
-        <v>1</v>
+        <v>289</v>
       </c>
       <c r="O98">
-        <v>1</v>
+        <v>289</v>
       </c>
       <c r="P98">
-        <v>1</v>
+        <v>289</v>
       </c>
       <c r="R98">
-        <v>1</v>
+        <v>289</v>
       </c>
       <c r="S98">
-        <v>1</v>
+        <v>289</v>
       </c>
       <c r="T98">
-        <v>1</v>
+        <v>289</v>
       </c>
       <c r="X98" s="2" t="s">
         <v>203</v>
@@ -5450,16 +5497,16 @@
         <v>228</v>
       </c>
       <c r="N99">
-        <v>1</v>
+        <v>292</v>
       </c>
       <c r="O99">
-        <v>1</v>
+        <v>292</v>
       </c>
       <c r="R99">
-        <v>1</v>
+        <v>292</v>
       </c>
       <c r="S99">
-        <v>1</v>
+        <v>292</v>
       </c>
       <c r="X99" s="2" t="s">
         <v>203</v>
@@ -5490,19 +5537,19 @@
         <v>19</v>
       </c>
       <c r="N100">
-        <v>1</v>
+        <v>295</v>
       </c>
       <c r="O100">
-        <v>1</v>
+        <v>295</v>
       </c>
       <c r="P100">
-        <v>1</v>
+        <v>295</v>
       </c>
       <c r="S100">
-        <v>1</v>
+        <v>295</v>
       </c>
       <c r="W100">
-        <v>1</v>
+        <v>295</v>
       </c>
       <c r="X100" t="s">
         <v>232</v>
@@ -5533,13 +5580,16 @@
         <v>349</v>
       </c>
       <c r="N101">
-        <v>1</v>
+        <v>298</v>
       </c>
       <c r="O101">
-        <v>1</v>
+        <v>298</v>
+      </c>
+      <c r="S101">
+        <v>298</v>
       </c>
       <c r="W101">
-        <v>1</v>
+        <v>298</v>
       </c>
       <c r="X101" t="s">
         <v>232</v>
@@ -5570,16 +5620,16 @@
         <v>39</v>
       </c>
       <c r="N102">
-        <v>1</v>
+        <v>301</v>
       </c>
       <c r="O102">
-        <v>1</v>
+        <v>301</v>
       </c>
       <c r="S102">
-        <v>1</v>
+        <v>301</v>
       </c>
       <c r="W102">
-        <v>1</v>
+        <v>301</v>
       </c>
       <c r="X102" t="s">
         <v>232</v>
@@ -5607,16 +5657,16 @@
         <v>69.95</v>
       </c>
       <c r="N103">
-        <v>1</v>
+        <v>304</v>
       </c>
       <c r="O103">
-        <v>1</v>
+        <v>304</v>
       </c>
       <c r="S103">
-        <v>1</v>
+        <v>304</v>
       </c>
       <c r="W103">
-        <v>1</v>
+        <v>304</v>
       </c>
       <c r="X103" t="s">
         <v>232</v>
@@ -5644,10 +5694,13 @@
         <v>799</v>
       </c>
       <c r="O104">
-        <v>1</v>
+        <v>307</v>
+      </c>
+      <c r="S104">
+        <v>307</v>
       </c>
       <c r="W104">
-        <v>1</v>
+        <v>307</v>
       </c>
       <c r="X104" t="s">
         <v>232</v>
@@ -5675,13 +5728,13 @@
         <v>69.95</v>
       </c>
       <c r="N105">
-        <v>1</v>
+        <v>310</v>
       </c>
       <c r="S105">
-        <v>1</v>
+        <v>310</v>
       </c>
       <c r="W105">
-        <v>1</v>
+        <v>310</v>
       </c>
       <c r="X105" t="s">
         <v>232</v>
@@ -5712,19 +5765,19 @@
         <v>120</v>
       </c>
       <c r="N106">
-        <v>1</v>
+        <v>313</v>
       </c>
       <c r="O106">
-        <v>1</v>
+        <v>313</v>
       </c>
       <c r="P106">
-        <v>1</v>
+        <v>313</v>
       </c>
       <c r="S106">
-        <v>1</v>
+        <v>313</v>
       </c>
       <c r="W106">
-        <v>1</v>
+        <v>313</v>
       </c>
       <c r="X106" t="s">
         <v>232</v>
@@ -5752,10 +5805,13 @@
         <v>599</v>
       </c>
       <c r="N107">
-        <v>1</v>
+        <v>316</v>
+      </c>
+      <c r="S107">
+        <v>316</v>
       </c>
       <c r="W107">
-        <v>1</v>
+        <v>316</v>
       </c>
       <c r="X107" t="s">
         <v>232</v>
@@ -5783,10 +5839,10 @@
         <v>69.95</v>
       </c>
       <c r="N108">
-        <v>1</v>
+        <v>319</v>
       </c>
       <c r="W108">
-        <v>1</v>
+        <v>319</v>
       </c>
       <c r="X108" t="s">
         <v>232</v>
@@ -5817,16 +5873,16 @@
         <v>179</v>
       </c>
       <c r="N109">
-        <v>1</v>
+        <v>322</v>
       </c>
       <c r="R109">
-        <v>1</v>
+        <v>322</v>
       </c>
       <c r="S109">
-        <v>1</v>
+        <v>322</v>
       </c>
       <c r="T109">
-        <v>1</v>
+        <v>322</v>
       </c>
       <c r="X109" t="s">
         <v>258</v>
@@ -5857,16 +5913,16 @@
         <v>175</v>
       </c>
       <c r="N110">
-        <v>1</v>
+        <v>325</v>
       </c>
       <c r="R110">
-        <v>1</v>
+        <v>325</v>
       </c>
       <c r="S110">
-        <v>1</v>
+        <v>325</v>
       </c>
       <c r="T110">
-        <v>1</v>
+        <v>325</v>
       </c>
       <c r="X110" t="s">
         <v>258</v>
@@ -5897,22 +5953,22 @@
         <v>384</v>
       </c>
       <c r="N111">
-        <v>1</v>
+        <v>328</v>
       </c>
       <c r="O111">
-        <v>1</v>
+        <v>328</v>
       </c>
       <c r="P111">
-        <v>1</v>
+        <v>328</v>
       </c>
       <c r="R111">
-        <v>1</v>
+        <v>328</v>
       </c>
       <c r="S111">
-        <v>1</v>
+        <v>328</v>
       </c>
       <c r="T111">
-        <v>1</v>
+        <v>328</v>
       </c>
       <c r="X111" t="s">
         <v>258</v>
@@ -5943,22 +5999,22 @@
         <v>385</v>
       </c>
       <c r="N112">
-        <v>1</v>
+        <v>331</v>
       </c>
       <c r="O112">
-        <v>1</v>
+        <v>331</v>
       </c>
       <c r="P112">
-        <v>1</v>
+        <v>331</v>
       </c>
       <c r="R112">
-        <v>1</v>
+        <v>331</v>
       </c>
       <c r="S112">
-        <v>1</v>
+        <v>331</v>
       </c>
       <c r="T112">
-        <v>1</v>
+        <v>331</v>
       </c>
       <c r="X112" t="s">
         <v>258</v>
@@ -5986,7 +6042,13 @@
         <v>399</v>
       </c>
       <c r="N113">
-        <v>1</v>
+        <v>334</v>
+      </c>
+      <c r="S113">
+        <v>334</v>
+      </c>
+      <c r="U113">
+        <v>334</v>
       </c>
       <c r="X113" t="s">
         <v>258</v>
@@ -6016,19 +6078,22 @@
         <v>45</v>
       </c>
       <c r="N114">
-        <v>1</v>
+        <v>337</v>
       </c>
       <c r="O114">
-        <v>1</v>
+        <v>337</v>
+      </c>
+      <c r="Q114">
+        <v>337</v>
       </c>
       <c r="R114">
-        <v>1</v>
+        <v>337</v>
       </c>
       <c r="S114">
-        <v>1</v>
+        <v>337</v>
       </c>
       <c r="T114">
-        <v>1</v>
+        <v>337</v>
       </c>
       <c r="X114" t="s">
         <v>258</v>
@@ -6058,19 +6123,25 @@
         <v>19</v>
       </c>
       <c r="N115">
-        <v>1</v>
+        <v>340</v>
       </c>
       <c r="O115">
-        <v>1</v>
+        <v>340</v>
       </c>
       <c r="P115">
-        <v>1</v>
+        <v>340</v>
+      </c>
+      <c r="Q115">
+        <v>340</v>
+      </c>
+      <c r="R115">
+        <v>340</v>
       </c>
       <c r="S115">
-        <v>1</v>
+        <v>340</v>
       </c>
       <c r="T115">
-        <v>1</v>
+        <v>340</v>
       </c>
       <c r="X115" t="s">
         <v>258</v>
@@ -6094,19 +6165,22 @@
         <v>19.95</v>
       </c>
       <c r="N116">
-        <v>1</v>
+        <v>343</v>
       </c>
       <c r="O116">
-        <v>1</v>
+        <v>343</v>
       </c>
       <c r="P116">
-        <v>1</v>
+        <v>343</v>
+      </c>
+      <c r="R116">
+        <v>343</v>
       </c>
       <c r="S116">
-        <v>1</v>
+        <v>343</v>
       </c>
       <c r="T116">
-        <v>1</v>
+        <v>343</v>
       </c>
       <c r="X116" t="s">
         <v>258</v>
@@ -6136,19 +6210,19 @@
         <v>69</v>
       </c>
       <c r="N117">
-        <v>1</v>
+        <v>346</v>
       </c>
       <c r="O117">
-        <v>1</v>
+        <v>346</v>
       </c>
       <c r="R117">
-        <v>1</v>
+        <v>346</v>
       </c>
       <c r="S117">
-        <v>1</v>
+        <v>346</v>
       </c>
       <c r="T117">
-        <v>1</v>
+        <v>346</v>
       </c>
       <c r="X117" t="s">
         <v>258</v>

</xml_diff>